<commit_message>
Filled in some missing actions
</commit_message>
<xml_diff>
--- a/Meta/flagsMap_withDecisions.xlsx
+++ b/Meta/flagsMap_withDecisions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa.sharepoint.com/sites/LakeMichiganML/Shared Documents/General/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="280" documentId="13_ncr:4000b_{6437034B-B068-4CF2-9A04-9208A97A6BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69764371-4A6D-4514-9EA3-547A12C6525E}"/>
+  <xr:revisionPtr revIDLastSave="293" documentId="13_ncr:4000b_{6437034B-B068-4CF2-9A04-9208A97A6BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF06E8CC-468A-4F57-BF60-4D3E92F2C46E}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="flagsMap_withDecisions" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,8 @@
 E=Estimated value (between MDL and RL or another issue)
 RL=Below RL
 ChlaF=WI State Lab of Hygiene flag for chl-a filter size
-C=Lab correction factor</t>
+C=Lab correction factor
+MDL_impute=MDL inferred as lowest result value reported by lab</t>
       </text>
     </comment>
     <comment ref="G1" authorId="1" shapeId="0" xr:uid="{9DD5E251-9F0E-49B4-8118-B96699C3281D}">
@@ -84,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="174">
   <si>
     <t>Study</t>
   </si>
@@ -545,9 +546,6 @@
     <t>Lab correction factor</t>
   </si>
   <si>
-    <t>Set value to NA; report RL in separate column. Note the Value is &lt;RL</t>
-  </si>
-  <si>
     <t>Invalid</t>
   </si>
   <si>
@@ -597,6 +595,18 @@
   </si>
   <si>
     <t>Likely will not be able to create this flag for NCCA_WChem_2010 because don't have lab flag, and don't want to flag all WI samples.</t>
+  </si>
+  <si>
+    <t>Set value to NA; report RL in separate column. Note the RL is contained in the Value as "&lt;RL"</t>
+  </si>
+  <si>
+    <t>MDL_impute</t>
+  </si>
+  <si>
+    <t>MDL imputed</t>
+  </si>
+  <si>
+    <t>Christian Filled these in. Needs verification</t>
   </si>
 </sst>
 </file>
@@ -1121,7 +1131,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1168,6 +1178,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1540,7 +1553,8 @@
 E=Estimated value (between MDL and RL or another issue)
 RL=Below RL
 ChlaF=WI State Lab of Hygiene flag for chl-a filter size
-C=Lab correction factor</text>
+C=Lab correction factor
+MDL_impute=MDL inferred as lowest result value reported by lab</text>
   </threadedComment>
   <threadedComment ref="G1" dT="2024-08-14T15:23:21.99" personId="{661D028C-1F83-4763-B7EC-DB616DE23CF1}" id="{9DD5E251-9F0E-49B4-8118-B96699C3281D}">
     <text>Keep=keep observations with this flag, no modifications necessary.
@@ -1563,8 +1577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="D8" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1668,7 +1682,7 @@
         <v>139</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1795,7 +1809,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>4</v>
       </c>
@@ -1803,12 +1817,16 @@
         <v>18</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="G11" s="13"/>
-      <c r="H11" s="11"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+        <v>156</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>4</v>
       </c>
@@ -1816,10 +1834,14 @@
         <v>15</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="G12" s="13"/>
-      <c r="H12" s="11"/>
+        <v>156</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="13" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
@@ -2049,7 +2071,7 @@
         <v>139</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2091,12 +2113,16 @@
       <c r="D26" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="E26" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>172</v>
+      </c>
       <c r="G26" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="H26" s="7" t="s">
-        <v>142</v>
-      </c>
+      <c r="H26" s="7"/>
     </row>
     <row r="27" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
@@ -2252,20 +2278,20 @@
         <v>94</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D34" s="9"/>
       <c r="E34" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="F34" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="F34" s="10" t="s">
-        <v>163</v>
-      </c>
       <c r="G34" s="15" t="s">
         <v>89</v>
       </c>
       <c r="H34" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="35" spans="1:20" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -2276,7 +2302,7 @@
         <v>51</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="7" t="s">
@@ -2312,7 +2338,7 @@
         <v>94</v>
       </c>
       <c r="C36" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>141</v>
@@ -2335,7 +2361,7 @@
         <v>94</v>
       </c>
       <c r="C37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>141</v>
@@ -2358,7 +2384,7 @@
         <v>94</v>
       </c>
       <c r="C38" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>141</v>
@@ -2381,7 +2407,7 @@
         <v>94</v>
       </c>
       <c r="C39" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D39" s="7" t="s">
         <v>141</v>
@@ -2404,7 +2430,7 @@
         <v>94</v>
       </c>
       <c r="C40" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>141</v>
@@ -2626,7 +2652,7 @@
         <v>139</v>
       </c>
       <c r="H48" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
@@ -2721,7 +2747,7 @@
         <v>139</v>
       </c>
       <c r="H52" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
@@ -2879,7 +2905,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A60" s="6" t="s">
         <v>52</v>
       </c>
@@ -2902,7 +2928,7 @@
         <v>139</v>
       </c>
       <c r="H60" s="12" t="s">
-        <v>153</v>
+        <v>170</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="52.2" x14ac:dyDescent="0.3">
@@ -3199,10 +3225,10 @@
         <v>53</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G74" s="16" t="s">
         <v>25</v>
@@ -3216,7 +3242,7 @@
         <v>53</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D75" s="3"/>
       <c r="G75" s="16" t="s">
@@ -3281,21 +3307,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100919AB8A12910594B8F4D80F4ACA7D0E7" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9c71394a73500791d9f4b659570ff6f6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a318c9bd-5828-4914-8ac9-a57d8c01df7a" xmlns:ns3="4da7f078-0f32-436f-b12a-21525bae5a0e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f0993cb8e7f28d1e7915cb051b812a71" ns2:_="" ns3:_="">
     <xsd:import namespace="a318c9bd-5828-4914-8ac9-a57d8c01df7a"/>
@@ -3472,24 +3483,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC4DE233-B05C-40D4-9E0D-B697BD35B3E3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B8261F5-E2C2-49F8-99F3-13EB69507EB7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56F0D49C-4924-48A7-977F-FB48DDC11B03}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3506,4 +3515,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B8261F5-E2C2-49F8-99F3-13EB69507EB7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC4DE233-B05C-40D4-9E0D-B697BD35B3E3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated to single letter codes and added MDL for CSMI2021
</commit_message>
<xml_diff>
--- a/Meta/flagsMap_withDecisions.xlsx
+++ b/Meta/flagsMap_withDecisions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa.sharepoint.com/sites/LakeMichiganML/Shared Documents/General/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="293" documentId="13_ncr:4000b_{6437034B-B068-4CF2-9A04-9208A97A6BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF06E8CC-468A-4F57-BF60-4D3E92F2C46E}"/>
+  <xr:revisionPtr revIDLastSave="341" documentId="13_ncr:4000b_{6437034B-B068-4CF2-9A04-9208A97A6BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{742A5774-88B6-4128-B965-21C16C5153E9}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="flagsMap_withDecisions" sheetId="1" r:id="rId1"/>
@@ -34,16 +34,16 @@
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    CTB=Secchi clear to bottom
+    B=Secchi clear to bottom
 U=Units imputed
-QC=lab or field QC issue
+Q=lab or field QC issue
 H=Holding time exceeded
-MDL=Below MDL
+N=Below MDL (nondetect)
 E=Estimated value (between MDL and RL or another issue)
-RL=Below RL
-ChlaF=WI State Lab of Hygiene flag for chl-a filter size
+R=Below RL
+F=WI State Lab of Hygiene flag for chl-a filter size
 C=Lab correction factor
-MDL_impute=MDL inferred as lowest result value reported by lab</t>
+L=MDL inferred as lowest result value reported by lab</t>
       </text>
     </comment>
     <comment ref="G1" authorId="1" shapeId="0" xr:uid="{9DD5E251-9F0E-49B4-8118-B96699C3281D}">
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="172">
   <si>
     <t>Study</t>
   </si>
@@ -444,15 +444,9 @@
     <t>Result value was not determined or entered for reasons other than those presented in this list. No result value was reported</t>
   </si>
   <si>
-    <t>QC</t>
-  </si>
-  <si>
     <t>QC issue</t>
   </si>
   <si>
-    <t>RL</t>
-  </si>
-  <si>
     <t>Reported value is probably biased low as evidenced by LMS (matrix spike, lab) results, SRM (reference material, standard) recovery or other internal lab QC data.  Reported value is not considered invalid, however</t>
   </si>
   <si>
@@ -570,9 +564,6 @@
     <t>Improper filter used.</t>
   </si>
   <si>
-    <t>ChlaF</t>
-  </si>
-  <si>
     <t>WSLH uses 5 micron pore size vs. NARS uses 0.7 micron for chl-a</t>
   </si>
   <si>
@@ -600,13 +591,16 @@
     <t>Set value to NA; report RL in separate column. Note the RL is contained in the Value as "&lt;RL"</t>
   </si>
   <si>
-    <t>MDL_impute</t>
-  </si>
-  <si>
     <t>MDL imputed</t>
   </si>
   <si>
     <t>Christian Filled these in. Needs verification</t>
+  </si>
+  <si>
+    <t>CSMI_2021</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -760,7 +754,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -967,6 +961,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1180,7 +1180,7 @@
     <xf numFmtId="0" fontId="19" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1545,16 +1545,16 @@
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <threadedComment ref="E1" dT="2024-08-14T15:27:31.24" personId="{661D028C-1F83-4763-B7EC-DB616DE23CF1}" id="{068A9404-2F3B-466F-9954-2FBC3269B52F}">
-    <text>CTB=Secchi clear to bottom
+    <text>B=Secchi clear to bottom
 U=Units imputed
-QC=lab or field QC issue
+Q=lab or field QC issue
 H=Holding time exceeded
-MDL=Below MDL
+N=Below MDL (nondetect)
 E=Estimated value (between MDL and RL or another issue)
-RL=Below RL
-ChlaF=WI State Lab of Hygiene flag for chl-a filter size
+R=Below RL
+F=WI State Lab of Hygiene flag for chl-a filter size
 C=Lab correction factor
-MDL_impute=MDL inferred as lowest result value reported by lab</text>
+L=MDL inferred as lowest result value reported by lab</text>
   </threadedComment>
   <threadedComment ref="G1" dT="2024-08-14T15:23:21.99" personId="{661D028C-1F83-4763-B7EC-DB616DE23CF1}" id="{9DD5E251-9F0E-49B4-8118-B96699C3281D}">
     <text>Keep=keep observations with this flag, no modifications necessary.
@@ -1577,8 +1577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D8" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="D71" workbookViewId="0">
+      <selection activeCell="F76" sqref="F76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1617,7 +1617,7 @@
         <v>88</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1628,7 +1628,7 @@
         <v>18</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>19</v>
@@ -1638,7 +1638,7 @@
         <v>25</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1649,7 +1649,7 @@
         <v>15</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>17</v>
@@ -1659,7 +1659,7 @@
         <v>25</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -1673,16 +1673,16 @@
         <v>6</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>6</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1702,13 +1702,13 @@
         <v>7</v>
       </c>
       <c r="F5" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="H5" s="6" t="s">
         <v>136</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1728,7 +1728,7 @@
         <v>89</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1748,7 +1748,7 @@
         <v>89</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -1786,7 +1786,7 @@
         <v>25</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1806,7 +1806,7 @@
         <v>25</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1817,13 +1817,13 @@
         <v>18</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G11" s="13" t="s">
         <v>25</v>
       </c>
       <c r="H11" s="18" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -1834,13 +1834,13 @@
         <v>15</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G12" s="13" t="s">
         <v>25</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
@@ -1919,7 +1919,7 @@
         <v>9</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>11</v>
@@ -1928,7 +1928,7 @@
         <v>25</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -1939,16 +1939,16 @@
         <v>21</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>22</v>
       </c>
       <c r="E18" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F18" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>120</v>
       </c>
       <c r="G18" s="17" t="s">
         <v>89</v>
@@ -1962,16 +1962,16 @@
         <v>21</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>22</v>
       </c>
       <c r="E19" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F19" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>120</v>
       </c>
       <c r="G19" s="17" t="s">
         <v>89</v>
@@ -2016,13 +2016,13 @@
         <v>7</v>
       </c>
       <c r="F22" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="H22" s="6" t="s">
         <v>136</v>
-      </c>
-      <c r="G22" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="H22" s="6" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2042,13 +2042,13 @@
         <v>7</v>
       </c>
       <c r="F23" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="H23" s="6" t="s">
         <v>136</v>
-      </c>
-      <c r="G23" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="H23" s="6" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
@@ -2062,16 +2062,16 @@
         <v>6</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>6</v>
       </c>
       <c r="G24" s="14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2088,16 +2088,16 @@
         <v>31</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>93</v>
+        <v>30</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G25" s="14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2114,10 +2114,10 @@
         <v>33</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>171</v>
+        <v>42</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="G26" s="15" t="s">
         <v>89</v>
@@ -2138,16 +2138,16 @@
         <v>35</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>93</v>
+        <v>30</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2167,7 +2167,7 @@
         <v>95</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G28" s="15" t="s">
         <v>89</v>
@@ -2184,10 +2184,10 @@
         <v>39</v>
       </c>
       <c r="E29" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F29" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>120</v>
       </c>
       <c r="G29" s="15" t="s">
         <v>89</v>
@@ -2247,7 +2247,7 @@
         <v>89</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="33" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
@@ -2261,10 +2261,10 @@
         <v>49</v>
       </c>
       <c r="E33" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F33" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>120</v>
       </c>
       <c r="G33" s="15" t="s">
         <v>89</v>
@@ -2278,20 +2278,20 @@
         <v>94</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D34" s="9"/>
       <c r="E34" s="10" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="G34" s="15" t="s">
         <v>89</v>
       </c>
       <c r="H34" s="12" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="35" spans="1:20" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -2302,20 +2302,20 @@
         <v>51</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="7" t="s">
-        <v>93</v>
+        <v>30</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G35" s="14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="I35" s="7"/>
       <c r="J35" s="7"/>
@@ -2338,16 +2338,16 @@
         <v>94</v>
       </c>
       <c r="C36" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E36" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F36" s="7" t="s">
         <v>119</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>120</v>
       </c>
       <c r="G36" s="15" t="s">
         <v>89</v>
@@ -2361,16 +2361,16 @@
         <v>94</v>
       </c>
       <c r="C37" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E37" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F37" s="7" t="s">
         <v>119</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>120</v>
       </c>
       <c r="G37" s="15" t="s">
         <v>89</v>
@@ -2384,16 +2384,16 @@
         <v>94</v>
       </c>
       <c r="C38" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E38" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F38" s="7" t="s">
         <v>119</v>
-      </c>
-      <c r="F38" s="7" t="s">
-        <v>120</v>
       </c>
       <c r="G38" s="15" t="s">
         <v>89</v>
@@ -2407,16 +2407,16 @@
         <v>94</v>
       </c>
       <c r="C39" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E39" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F39" s="7" t="s">
         <v>119</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>120</v>
       </c>
       <c r="G39" s="15" t="s">
         <v>89</v>
@@ -2430,16 +2430,16 @@
         <v>94</v>
       </c>
       <c r="C40" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E40" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F40" s="7" t="s">
         <v>119</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>120</v>
       </c>
       <c r="G40" s="15" t="s">
         <v>89</v>
@@ -2460,7 +2460,7 @@
         <v>95</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G41" s="15" t="s">
         <v>89</v>
@@ -2488,7 +2488,7 @@
       </c>
       <c r="C42" s="7"/>
       <c r="D42" s="7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E42" s="7" t="s">
         <v>92</v>
@@ -2527,10 +2527,10 @@
         <v>101</v>
       </c>
       <c r="E43" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F43" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>120</v>
       </c>
       <c r="G43" s="15" t="s">
         <v>89</v>
@@ -2551,10 +2551,10 @@
         <v>102</v>
       </c>
       <c r="E44" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F44" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>120</v>
       </c>
       <c r="G44" s="15" t="s">
         <v>89</v>
@@ -2597,10 +2597,10 @@
         <v>103</v>
       </c>
       <c r="E46" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F46" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="F46" s="6" t="s">
-        <v>120</v>
       </c>
       <c r="G46" s="15" t="s">
         <v>89</v>
@@ -2620,10 +2620,10 @@
         <v>104</v>
       </c>
       <c r="E47" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F47" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="F47" s="6" t="s">
-        <v>120</v>
       </c>
       <c r="G47" s="15" t="s">
         <v>89</v>
@@ -2643,16 +2643,16 @@
         <v>105</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>93</v>
+        <v>30</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G48" s="14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H48" s="12" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
@@ -2669,10 +2669,10 @@
         <v>106</v>
       </c>
       <c r="E49" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F49" s="7" t="s">
         <v>119</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>120</v>
       </c>
       <c r="G49" s="15" t="s">
         <v>89</v>
@@ -2692,10 +2692,10 @@
         <v>107</v>
       </c>
       <c r="E50" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F50" s="7" t="s">
         <v>119</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>120</v>
       </c>
       <c r="G50" s="15" t="s">
         <v>89</v>
@@ -2718,7 +2718,7 @@
         <v>95</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G51" s="15" t="s">
         <v>89</v>
@@ -2741,13 +2741,13 @@
         <v>96</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G52" s="14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H52" s="12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
@@ -2764,10 +2764,10 @@
         <v>109</v>
       </c>
       <c r="E53" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F53" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="F53" s="6" t="s">
-        <v>120</v>
       </c>
       <c r="G53" s="15" t="s">
         <v>89</v>
@@ -2787,10 +2787,10 @@
         <v>110</v>
       </c>
       <c r="E54" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F54" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="F54" s="6" t="s">
-        <v>120</v>
       </c>
       <c r="G54" s="15" t="s">
         <v>89</v>
@@ -2810,10 +2810,10 @@
         <v>111</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G55" s="15" t="s">
         <v>89</v>
@@ -2833,10 +2833,10 @@
         <v>112</v>
       </c>
       <c r="E56" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F56" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="F56" s="6" t="s">
-        <v>120</v>
       </c>
       <c r="G56" s="15" t="s">
         <v>89</v>
@@ -2856,10 +2856,10 @@
         <v>113</v>
       </c>
       <c r="E57" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F57" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="F57" s="6" t="s">
-        <v>120</v>
       </c>
       <c r="G57" s="15" t="s">
         <v>89</v>
@@ -2896,10 +2896,10 @@
         <v>115</v>
       </c>
       <c r="E59" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F59" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="F59" s="6" t="s">
-        <v>120</v>
       </c>
       <c r="G59" s="15" t="s">
         <v>89</v>
@@ -2919,16 +2919,16 @@
         <v>100</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>121</v>
+        <v>15</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G60" s="14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H60" s="12" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="52.2" x14ac:dyDescent="0.3">
@@ -2945,10 +2945,10 @@
         <v>116</v>
       </c>
       <c r="E61" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F61" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="F61" s="6" t="s">
-        <v>120</v>
       </c>
       <c r="G61" s="15" t="s">
         <v>89</v>
@@ -2968,10 +2968,10 @@
         <v>117</v>
       </c>
       <c r="E62" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F62" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="F62" s="6" t="s">
-        <v>120</v>
       </c>
       <c r="G62" s="15" t="s">
         <v>89</v>
@@ -3005,13 +3005,13 @@
         <v>75</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E64" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F64" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="F64" s="6" t="s">
-        <v>120</v>
       </c>
       <c r="G64" s="15" t="s">
         <v>89</v>
@@ -3028,13 +3028,13 @@
         <v>76</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E65" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F65" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="F65" s="6" t="s">
-        <v>120</v>
       </c>
       <c r="G65" s="15" t="s">
         <v>89</v>
@@ -3057,13 +3057,13 @@
         <v>95</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G66" s="15" t="s">
         <v>89</v>
       </c>
       <c r="H66" s="12" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
@@ -3077,13 +3077,13 @@
         <v>78</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E67" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F67" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="F67" s="6" t="s">
-        <v>120</v>
       </c>
       <c r="G67" s="15" t="s">
         <v>89</v>
@@ -3100,13 +3100,13 @@
         <v>79</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E68" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F68" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="F68" s="6" t="s">
-        <v>120</v>
       </c>
       <c r="G68" s="15" t="s">
         <v>89</v>
@@ -3123,13 +3123,13 @@
         <v>80</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E69" s="7" t="s">
         <v>95</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G69" s="15" t="s">
         <v>89</v>
@@ -3146,7 +3146,7 @@
         <v>81</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E70" s="7"/>
       <c r="F70" s="7"/>
@@ -3165,13 +3165,13 @@
         <v>82</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E71" s="7" t="s">
         <v>95</v>
       </c>
       <c r="F71" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G71" s="15" t="s">
         <v>89</v>
@@ -3188,7 +3188,7 @@
         <v>83</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G72" s="16" t="s">
         <v>25</v>
@@ -3205,13 +3205,13 @@
         <v>84</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E73" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F73" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="F73" s="6" t="s">
-        <v>120</v>
       </c>
       <c r="G73" s="15" t="s">
         <v>89</v>
@@ -3225,10 +3225,10 @@
         <v>53</v>
       </c>
       <c r="C74" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="D74" s="3" t="s">
         <v>153</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>155</v>
       </c>
       <c r="G74" s="16" t="s">
         <v>25</v>
@@ -3242,7 +3242,7 @@
         <v>53</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D75" s="3"/>
       <c r="G75" s="16" t="s">
@@ -3260,13 +3260,13 @@
         <v>85</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E76" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F76" s="6" t="s">
         <v>119</v>
-      </c>
-      <c r="F76" s="6" t="s">
-        <v>120</v>
       </c>
       <c r="G76" s="15" t="s">
         <v>89</v>
@@ -3284,16 +3284,40 @@
       </c>
       <c r="D77" s="5"/>
       <c r="E77" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F77" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="G77" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="H77" s="7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A78" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D78" s="5"/>
+      <c r="E78" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="F77" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="G77" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="H77" s="7" t="s">
-        <v>145</v>
+      <c r="F78" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="G78" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="H78" s="7" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added the MDL flag to map to unified
</commit_message>
<xml_diff>
--- a/Meta/flagsMap_withDecisions.xlsx
+++ b/Meta/flagsMap_withDecisions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa.sharepoint.com/sites/LakeMichiganML/Shared Documents/General/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="359" documentId="13_ncr:4000b_{6437034B-B068-4CF2-9A04-9208A97A6BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A20C3BD-1E1E-4EC8-8A89-6CBF35F17ADA}"/>
+  <xr:revisionPtr revIDLastSave="435" documentId="13_ncr:4000b_{6437034B-B068-4CF2-9A04-9208A97A6BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27FBB21C-BC71-440A-9EF0-10776B26F204}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="flagsMap_withDecisions" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <author>tc={068A9404-2F3B-466F-9954-2FBC3269B52F}</author>
     <author>tc={9DD5E251-9F0E-49B4-8118-B96699C3281D}</author>
     <author>tc={57535352-09AF-42AB-BEBD-584FAEC623BD}</author>
+    <author>tc={907734F2-7127-48D9-8E0B-8B1C2E203CA7}</author>
     <author>tc={A8BE5C20-40BD-42DF-838C-01B7D5AFF883}</author>
     <author>tc={6A749074-B681-48EE-9D60-AAD094A450F9}</author>
   </authors>
@@ -64,7 +65,15 @@
     Any actions required or anything not straightforward about the mapping</t>
       </text>
     </comment>
-    <comment ref="A2" authorId="3" shapeId="0" xr:uid="{A8BE5C20-40BD-42DF-838C-01B7D5AFF883}">
+    <comment ref="A6" authorId="3" shapeId="0" xr:uid="{907734F2-7127-48D9-8E0B-8B1C2E203CA7}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Note: Did not include 3 extra flags in current flagsMap.csv here with repeat QAcomment in QAcode</t>
+      </text>
+    </comment>
+    <comment ref="A11" authorId="4" shapeId="0" xr:uid="{A8BE5C20-40BD-42DF-838C-01B7D5AFF883}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -72,7 +81,7 @@
     In current flagsMap.csv, did not include R-no reported units because should go with U (row 47). Did not include Q10,R-recorded mean secchi depth is greater than station depth because it's for NC, not GL.</t>
       </text>
     </comment>
-    <comment ref="A25" authorId="4" shapeId="0" xr:uid="{6A749074-B681-48EE-9D60-AAD094A450F9}">
+    <comment ref="A34" authorId="5" shapeId="0" xr:uid="{6A749074-B681-48EE-9D60-AAD094A450F9}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -85,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="170">
   <si>
     <t>Study</t>
   </si>
@@ -589,13 +598,19 @@
   </si>
   <si>
     <t>Below Method Detection Limit or Unspecified Detection Limit</t>
+  </si>
+  <si>
+    <t>MDL</t>
+  </si>
+  <si>
+    <t>below MDL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -740,6 +755,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="38">
@@ -1543,10 +1564,13 @@
   <threadedComment ref="H1" dT="2024-08-14T15:38:04.47" personId="{661D028C-1F83-4763-B7EC-DB616DE23CF1}" id="{57535352-09AF-42AB-BEBD-584FAEC623BD}">
     <text>Any actions required or anything not straightforward about the mapping</text>
   </threadedComment>
-  <threadedComment ref="A2" dT="2024-08-14T17:33:35.12" personId="{661D028C-1F83-4763-B7EC-DB616DE23CF1}" id="{A8BE5C20-40BD-42DF-838C-01B7D5AFF883}">
+  <threadedComment ref="A6" dT="2024-08-14T17:05:26.53" personId="{661D028C-1F83-4763-B7EC-DB616DE23CF1}" id="{907734F2-7127-48D9-8E0B-8B1C2E203CA7}">
+    <text>Note: Did not include 3 extra flags in current flagsMap.csv here with repeat QAcomment in QAcode</text>
+  </threadedComment>
+  <threadedComment ref="A11" dT="2024-08-14T17:33:35.12" personId="{661D028C-1F83-4763-B7EC-DB616DE23CF1}" id="{A8BE5C20-40BD-42DF-838C-01B7D5AFF883}">
     <text>In current flagsMap.csv, did not include R-no reported units because should go with U (row 47). Did not include Q10,R-recorded mean secchi depth is greater than station depth because it's for NC, not GL.</text>
   </threadedComment>
-  <threadedComment ref="A25" dT="2024-08-14T17:05:26.53" personId="{661D028C-1F83-4763-B7EC-DB616DE23CF1}" id="{6A749074-B681-48EE-9D60-AAD094A450F9}">
+  <threadedComment ref="A34" dT="2024-08-14T17:05:26.53" personId="{661D028C-1F83-4763-B7EC-DB616DE23CF1}" id="{6A749074-B681-48EE-9D60-AAD094A450F9}">
     <text>Note: Did not include 3 extra flags in current flagsMap.csv here with repeat QAcomment in QAcode</text>
   </threadedComment>
 </ThreadedComments>
@@ -1554,26 +1578,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T79"/>
+  <dimension ref="A1:T88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H68" sqref="H68"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="44.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="38.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="44.33203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="38.5546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="15" style="6" customWidth="1"/>
     <col min="6" max="6" width="26" style="6" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="35.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="6"/>
+    <col min="7" max="7" width="10.5546875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="35.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1599,192 +1621,241 @@
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>4</v>
+    <row r="2" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>86</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>140</v>
+        <v>168</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>168</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>5</v>
+        <v>168</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>168</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>6</v>
+        <v>169</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>6</v>
+        <v>30</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>167</v>
       </c>
       <c r="G4" s="13" t="s">
         <v>132</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>4</v>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>50</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>8</v>
+        <v>168</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>169</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>130</v>
+        <v>30</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>167</v>
       </c>
       <c r="G5" s="13" t="s">
         <v>132</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>9</v>
+        <v>168</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>10</v>
+        <v>168</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>9</v>
+        <v>168</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>12</v>
+        <v>168</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>21</v>
+        <v>168</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="H8" s="7"/>
-    </row>
-    <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>9</v>
+        <v>168</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>13</v>
+        <v>168</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="H9" s="7"/>
-    </row>
-    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>9</v>
+        <v>168</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>14</v>
+        <v>168</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="H10" s="7"/>
-    </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>4</v>
       </c>
@@ -1792,856 +1863,808 @@
         <v>18</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11" s="17" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="7"/>
+      <c r="G11" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>149</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="7"/>
       <c r="G12" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="H12" s="17" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="H12" s="7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G16" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17" s="7"/>
+    </row>
+    <row r="18" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C18" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="H18" s="7"/>
+    </row>
+    <row r="19" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="H19" s="7"/>
+    </row>
+    <row r="20" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="H21" s="17" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D26" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G17" s="15" t="s">
+      <c r="G26" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="H26" s="11" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B27" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C27" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D27" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E27" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F27" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="G18" s="16" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="G27" s="16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B28" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C28" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D28" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="6" t="s">
+      <c r="E28" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F28" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="G19" s="16" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="G28" s="16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C29" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G20" s="15" t="s">
+      <c r="G29" s="15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C30" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G21" s="15" t="s">
+      <c r="G30" s="15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+    <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B31" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C31" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D31" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="6" t="s">
+      <c r="E31" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F31" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="G22" s="13" t="s">
+      <c r="G31" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="H22" s="6" t="s">
+      <c r="H31" s="6" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+    <row r="32" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B32" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C32" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D32" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E32" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F32" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="G23" s="13" t="s">
+      <c r="G32" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="H23" s="6" t="s">
+      <c r="H32" s="6" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A33" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B33" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C33" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E33" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="F33" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G24" s="13" t="s">
+      <c r="G33" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="H24" s="6" t="s">
+      <c r="H33" s="6" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+    <row r="34" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A34" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B34" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C34" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D34" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="E34" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F25" s="7" t="s">
+      <c r="F34" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="G25" s="13" t="s">
+      <c r="G34" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="H25" s="6" t="s">
+      <c r="H34" s="6" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+    <row r="35" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B35" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C35" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="E35" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F26" s="6" t="s">
+      <c r="F35" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="G26" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="H26" s="7"/>
-    </row>
-    <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+      <c r="G35" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="H35" s="7"/>
+    </row>
+    <row r="36" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A36" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B36" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C36" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D36" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E36" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F27" s="7" t="s">
+      <c r="F36" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="G27" s="13" t="s">
+      <c r="G36" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="H27" s="6" t="s">
+      <c r="H36" s="6" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+    <row r="37" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A37" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B37" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="C37" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="D37" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="E37" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="F37" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="G28" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+      <c r="G37" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A38" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B38" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C38" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="E38" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="F29" s="6" t="s">
+      <c r="F38" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="G29" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+      <c r="G38" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A39" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B39" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C39" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E30" s="6" t="s">
+      <c r="E39" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F39" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G30" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+      <c r="G39" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B40" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C40" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="G31" s="15" t="s">
+      <c r="G40" s="15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A41" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B41" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C41" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D41" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G32" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="H32" s="7" t="s">
+      <c r="G41" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="H41" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
+    <row r="42" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A42" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B42" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C42" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E33" s="6" t="s">
+      <c r="E42" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="F33" s="6" t="s">
+      <c r="F42" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="G33" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A34" s="10" t="s">
+      <c r="G42" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="B43" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C43" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="D34" s="9"/>
-      <c r="E34" s="10" t="s">
+      <c r="D43" s="9"/>
+      <c r="E43" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="F34" s="10" t="s">
+      <c r="F43" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="G34" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="H34" s="7" t="s">
+      <c r="G43" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="H43" s="7" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="35" spans="1:20" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
+    <row r="44" spans="1:20" s="10" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A44" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B44" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C44" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="D35" s="5"/>
-      <c r="E35" s="7" t="s">
+      <c r="D44" s="5"/>
+      <c r="E44" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F35" s="7" t="s">
+      <c r="F44" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="G35" s="13" t="s">
+      <c r="G44" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="H35" s="7" t="s">
+      <c r="H44" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="I35" s="7"/>
-      <c r="J35" s="7"/>
-      <c r="K35" s="7"/>
-      <c r="L35" s="7"/>
-      <c r="M35" s="7"/>
-      <c r="N35" s="7"/>
-      <c r="O35" s="7"/>
-      <c r="P35" s="7"/>
-      <c r="Q35" s="7"/>
-      <c r="R35" s="7"/>
-      <c r="S35" s="7"/>
-      <c r="T35" s="7"/>
-    </row>
-    <row r="36" spans="1:20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="I44" s="7"/>
+      <c r="J44" s="7"/>
+      <c r="K44" s="7"/>
+      <c r="L44" s="7"/>
+      <c r="M44" s="7"/>
+      <c r="N44" s="7"/>
+      <c r="O44" s="7"/>
+      <c r="P44" s="7"/>
+      <c r="Q44" s="7"/>
+      <c r="R44" s="7"/>
+      <c r="S44" s="7"/>
+      <c r="T44" s="7"/>
+    </row>
+    <row r="45" spans="1:20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>50</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B45" t="s">
         <v>93</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C45" t="s">
         <v>155</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D45" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="E36" s="7" t="s">
+      <c r="E45" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="F36" s="7" t="s">
+      <c r="F45" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="G36" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="G45" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>50</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B46" t="s">
         <v>93</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C46" t="s">
         <v>156</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D46" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="E37" s="7" t="s">
+      <c r="E46" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="F37" s="7" t="s">
+      <c r="F46" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="G37" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="G46" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>50</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B47" t="s">
         <v>93</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C47" t="s">
         <v>157</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D47" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="E38" s="7" t="s">
+      <c r="E47" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="F38" s="7" t="s">
+      <c r="F47" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="G38" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="G47" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>50</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B48" t="s">
         <v>93</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C48" t="s">
         <v>158</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D48" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="E39" s="7" t="s">
+      <c r="E48" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="F39" s="7" t="s">
+      <c r="F48" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="G39" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="G48" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>50</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B49" t="s">
         <v>93</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C49" t="s">
         <v>159</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D49" s="7" t="s">
         <v>134</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="G40" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="G41" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="H41" s="7"/>
-      <c r="I41" s="7"/>
-      <c r="J41" s="7"/>
-      <c r="K41" s="7"/>
-      <c r="L41" s="7"/>
-      <c r="M41" s="7"/>
-      <c r="N41" s="7"/>
-      <c r="O41" s="7"/>
-      <c r="P41" s="7"/>
-      <c r="Q41" s="7"/>
-      <c r="R41" s="7"/>
-      <c r="S41" s="7"/>
-      <c r="T41" s="7"/>
-    </row>
-    <row r="42" spans="1:20" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G42" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="H42" s="7"/>
-      <c r="I42" s="7"/>
-      <c r="J42" s="7"/>
-      <c r="K42" s="7"/>
-      <c r="L42" s="7"/>
-      <c r="M42" s="7"/>
-      <c r="N42" s="7"/>
-      <c r="O42" s="7"/>
-      <c r="P42" s="7"/>
-      <c r="Q42" s="7"/>
-      <c r="R42" s="7"/>
-      <c r="S42" s="7"/>
-      <c r="T42" s="7"/>
-    </row>
-    <row r="43" spans="1:20" ht="45.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="G43" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="H43" s="7"/>
-    </row>
-    <row r="44" spans="1:20" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="G44" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="45" spans="1:20" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G45" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="46" spans="1:20" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B46" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E46" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F46" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="G46" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="47" spans="1:20" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A47" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B47" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="E47" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F47" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="G47" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="48" spans="1:20" ht="165" x14ac:dyDescent="0.25">
-      <c r="A48" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B48" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C48" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E48" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F48" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="G48" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="H48" s="7" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A49" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B49" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="E49" s="7" t="s">
         <v>93</v>
@@ -2653,53 +2676,75 @@
         <v>89</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B50" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>105</v>
-      </c>
+    <row r="50" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D50" s="7"/>
       <c r="E50" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="G50" s="14" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A51" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B51" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>95</v>
+      <c r="H50" s="7"/>
+      <c r="I50" s="7"/>
+      <c r="J50" s="7"/>
+      <c r="K50" s="7"/>
+      <c r="L50" s="7"/>
+      <c r="M50" s="7"/>
+      <c r="N50" s="7"/>
+      <c r="O50" s="7"/>
+      <c r="P50" s="7"/>
+      <c r="Q50" s="7"/>
+      <c r="R50" s="7"/>
+      <c r="S50" s="7"/>
+      <c r="T50" s="7"/>
+    </row>
+    <row r="51" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C51" s="7"/>
+      <c r="D51" s="7" t="s">
+        <v>133</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>128</v>
+        <v>41</v>
       </c>
       <c r="G51" s="14" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="H51" s="7"/>
+      <c r="I51" s="7"/>
+      <c r="J51" s="7"/>
+      <c r="K51" s="7"/>
+      <c r="L51" s="7"/>
+      <c r="M51" s="7"/>
+      <c r="N51" s="7"/>
+      <c r="O51" s="7"/>
+      <c r="P51" s="7"/>
+      <c r="Q51" s="7"/>
+      <c r="R51" s="7"/>
+      <c r="S51" s="7"/>
+      <c r="T51" s="7"/>
+    </row>
+    <row r="52" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A52" s="6" t="s">
         <v>52</v>
       </c>
@@ -2707,25 +2752,23 @@
         <v>53</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E52" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F52" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="G52" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="H52" s="7" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G52" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="H52" s="7"/>
+    </row>
+    <row r="53" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A53" s="6" t="s">
         <v>52</v>
       </c>
@@ -2733,10 +2776,10 @@
         <v>53</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="E53" s="6" t="s">
         <v>93</v>
@@ -2748,7 +2791,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
         <v>52</v>
       </c>
@@ -2756,22 +2799,22 @@
         <v>53</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F54" s="6" t="s">
-        <v>117</v>
+        <v>92</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="G54" s="14" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
         <v>52</v>
       </c>
@@ -2779,22 +2822,22 @@
         <v>53</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>144</v>
+        <v>93</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="G55" s="14" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A56" s="6" t="s">
         <v>52</v>
       </c>
@@ -2802,10 +2845,10 @@
         <v>53</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="E56" s="6" t="s">
         <v>93</v>
@@ -2817,7 +2860,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A57" s="6" t="s">
         <v>52</v>
       </c>
@@ -2825,22 +2868,25 @@
         <v>53</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E57" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F57" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="G57" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="G57" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="H57" s="7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A58" s="6" t="s">
         <v>52</v>
       </c>
@@ -2848,16 +2894,22 @@
         <v>53</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G58" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="E58" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="G58" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A59" s="6" t="s">
         <v>52</v>
       </c>
@@ -2865,22 +2917,22 @@
         <v>53</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E59" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E59" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="F59" s="6" t="s">
+      <c r="F59" s="7" t="s">
         <v>117</v>
       </c>
       <c r="G59" s="14" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="45.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A60" s="6" t="s">
         <v>52</v>
       </c>
@@ -2888,25 +2940,22 @@
         <v>53</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>15</v>
+        <v>94</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="G60" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="H60" s="7" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+      <c r="G60" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A61" s="6" t="s">
         <v>52</v>
       </c>
@@ -2914,22 +2963,25 @@
         <v>53</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E61" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F61" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="G61" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="E61" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F61" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="G61" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="H61" s="7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A62" s="6" t="s">
         <v>52</v>
       </c>
@@ -2937,10 +2989,10 @@
         <v>53</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>115</v>
+        <v>64</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="E62" s="6" t="s">
         <v>93</v>
@@ -2952,7 +3004,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A63" s="6" t="s">
         <v>52</v>
       </c>
@@ -2960,16 +3012,22 @@
         <v>53</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="G63" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F63" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G63" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A64" s="6" t="s">
         <v>52</v>
       </c>
@@ -2977,22 +3035,22 @@
         <v>53</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>118</v>
+        <v>66</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>93</v>
+        <v>144</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>117</v>
+        <v>145</v>
       </c>
       <c r="G64" s="14" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A65" s="6" t="s">
         <v>52</v>
       </c>
@@ -3000,10 +3058,10 @@
         <v>53</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>119</v>
+        <v>67</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="E65" s="6" t="s">
         <v>93</v>
@@ -3015,7 +3073,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A66" s="6" t="s">
         <v>52</v>
       </c>
@@ -3023,25 +3081,22 @@
         <v>53</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="E66" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F66" s="7" t="s">
-        <v>128</v>
+        <v>111</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F66" s="6" t="s">
+        <v>117</v>
       </c>
       <c r="G66" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="H66" s="7" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:8" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A67" s="6" t="s">
         <v>52</v>
       </c>
@@ -3049,22 +3104,16 @@
         <v>53</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="E67" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F67" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="G67" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="G67" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A68" s="6" t="s">
         <v>52</v>
       </c>
@@ -3072,10 +3121,10 @@
         <v>53</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>121</v>
+        <v>70</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="E68" s="6" t="s">
         <v>93</v>
@@ -3087,7 +3136,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A69" s="6" t="s">
         <v>52</v>
       </c>
@@ -3095,22 +3144,25 @@
         <v>53</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>122</v>
+        <v>71</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>98</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>94</v>
+        <v>15</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="G69" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="G69" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="H69" s="7" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="52.2" x14ac:dyDescent="0.3">
       <c r="A70" s="6" t="s">
         <v>52</v>
       </c>
@@ -3118,18 +3170,22 @@
         <v>53</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="E70" s="7"/>
-      <c r="F70" s="7"/>
-      <c r="G70" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F70" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G70" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A71" s="6" t="s">
         <v>52</v>
       </c>
@@ -3137,22 +3193,22 @@
         <v>53</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="E71" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F71" s="7" t="s">
-        <v>128</v>
+        <v>115</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F71" s="6" t="s">
+        <v>117</v>
       </c>
       <c r="G71" s="14" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A72" s="6" t="s">
         <v>52</v>
       </c>
@@ -3160,16 +3216,16 @@
         <v>53</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="G72" s="15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="45.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" ht="42" x14ac:dyDescent="0.3">
       <c r="A73" s="6" t="s">
         <v>52</v>
       </c>
@@ -3177,10 +3233,10 @@
         <v>53</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="E73" s="6" t="s">
         <v>93</v>
@@ -3192,7 +3248,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A74" s="6" t="s">
         <v>52</v>
       </c>
@@ -3200,16 +3256,22 @@
         <v>53</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>146</v>
+        <v>76</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="G74" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="E74" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F74" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G74" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A75" s="6" t="s">
         <v>52</v>
       </c>
@@ -3217,14 +3279,25 @@
         <v>53</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="D75" s="3"/>
-      <c r="G75" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E75" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F75" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G75" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="H75" s="7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A76" s="6" t="s">
         <v>52</v>
       </c>
@@ -3232,10 +3305,10 @@
         <v>53</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="E76" s="6" t="s">
         <v>93</v>
@@ -3247,56 +3320,239 @@
         <v>89</v>
       </c>
     </row>
-    <row r="77" spans="1:8" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A77" s="7" t="s">
+    <row r="77" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
+      <c r="A77" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E77" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F77" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G77" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
+      <c r="A78" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E78" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F78" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G78" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
+      <c r="A79" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E79" s="7"/>
+      <c r="F79" s="7"/>
+      <c r="G79" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="21.6" x14ac:dyDescent="0.3">
+      <c r="A80" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B80" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E80" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F80" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G80" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
+      <c r="A81" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G81" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+      <c r="A82" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B82" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E82" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F82" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G82" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A83" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="G83" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A84" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="D84" s="3"/>
+      <c r="G84" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
+      <c r="A85" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E85" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F85" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G85" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A86" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="B77" s="7" t="s">
+      <c r="B86" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C77" s="7" t="s">
+      <c r="C86" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D77" s="5"/>
-      <c r="E77" s="7" t="s">
+      <c r="D86" s="5"/>
+      <c r="E86" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F77" s="7" t="s">
+      <c r="F86" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="G77" s="13" t="s">
+      <c r="G86" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="H77" s="7" t="s">
+      <c r="H86" s="7" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="78" spans="1:8" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A78" s="7" t="s">
+    <row r="87" spans="1:8" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A87" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="B78" s="7" t="s">
+      <c r="B87" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C78" s="7" t="s">
+      <c r="C87" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D78" s="5"/>
-      <c r="E78" s="7" t="s">
+      <c r="D87" s="5"/>
+      <c r="E87" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F78" s="7" t="s">
+      <c r="F87" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="G78" s="13" t="s">
+      <c r="G87" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="H78" s="7" t="s">
+      <c r="H87" s="7" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C79" s="7"/>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C88" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added qa flag for imputing time in glenda to noon
</commit_message>
<xml_diff>
--- a/Meta/flagsMap_withDecisions.xlsx
+++ b/Meta/flagsMap_withDecisions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa.sharepoint.com/sites/LakeMichiganML/Shared Documents/General/Results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/coffman_christian_epa_gov/Documents/Profile/Documents/Projects/GL_Data/Meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="435" documentId="13_ncr:4000b_{6437034B-B068-4CF2-9A04-9208A97A6BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27FBB21C-BC71-440A-9EF0-10776B26F204}"/>
+  <xr:revisionPtr revIDLastSave="440" documentId="13_ncr:4000b_{6437034B-B068-4CF2-9A04-9208A97A6BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2DD346F7-97AE-43BB-BD74-162FA987B8CD}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="flagsMap_withDecisions" sheetId="1" r:id="rId1"/>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="174">
   <si>
     <t>Study</t>
   </si>
@@ -604,13 +604,25 @@
   </si>
   <si>
     <t>below MDL</t>
+  </si>
+  <si>
+    <t>sample time imputed as noon</t>
+  </si>
+  <si>
+    <t>sample time reported so we filled it in guessing it was 12 noon</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>time issue</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -755,12 +767,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="38">
@@ -1578,9 +1584,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T88"/>
+  <dimension ref="A1:T89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2744,7 +2752,7 @@
       <c r="S51" s="7"/>
       <c r="T51" s="7"/>
     </row>
-    <row r="52" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A52" s="6" t="s">
         <v>52</v>
       </c>
@@ -2752,16 +2760,16 @@
         <v>53</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>54</v>
+        <v>170</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>99</v>
+        <v>171</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>93</v>
+        <v>172</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>117</v>
+        <v>173</v>
       </c>
       <c r="G52" s="14" t="s">
         <v>89</v>
@@ -2776,10 +2784,10 @@
         <v>53</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E53" s="6" t="s">
         <v>93</v>
@@ -2790,6 +2798,7 @@
       <c r="G53" s="14" t="s">
         <v>89</v>
       </c>
+      <c r="H53" s="7"/>
     </row>
     <row r="54" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
@@ -2799,16 +2808,16 @@
         <v>53</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>41</v>
+        <v>93</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>117</v>
       </c>
       <c r="G54" s="14" t="s">
         <v>89</v>
@@ -2822,16 +2831,16 @@
         <v>53</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F55" s="6" t="s">
-        <v>117</v>
+        <v>92</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="G55" s="14" t="s">
         <v>89</v>
@@ -2845,10 +2854,10 @@
         <v>53</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E56" s="6" t="s">
         <v>93</v>
@@ -2860,7 +2869,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A57" s="6" t="s">
         <v>52</v>
       </c>
@@ -2868,25 +2877,22 @@
         <v>53</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E57" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F57" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="G57" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="H57" s="7" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="58" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G57" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A58" s="6" t="s">
         <v>52</v>
       </c>
@@ -2894,19 +2900,22 @@
         <v>53</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>93</v>
+        <v>30</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="G58" s="14" t="s">
-        <v>89</v>
+        <v>167</v>
+      </c>
+      <c r="G58" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="H58" s="7" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="59" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
@@ -2917,10 +2926,10 @@
         <v>53</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E59" s="7" t="s">
         <v>93</v>
@@ -2932,7 +2941,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A60" s="6" t="s">
         <v>52</v>
       </c>
@@ -2940,22 +2949,22 @@
         <v>53</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="G60" s="14" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="61" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:20" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A61" s="6" t="s">
         <v>52</v>
       </c>
@@ -2963,25 +2972,22 @@
         <v>53</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>30</v>
+        <v>94</v>
       </c>
       <c r="F61" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="G61" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="H61" s="7" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="62" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+      <c r="G61" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A62" s="6" t="s">
         <v>52</v>
       </c>
@@ -2989,19 +2995,22 @@
         <v>53</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E62" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F62" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="G62" s="14" t="s">
-        <v>89</v>
+        <v>106</v>
+      </c>
+      <c r="E62" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F62" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="G62" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="H62" s="7" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="63" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
@@ -3012,10 +3021,10 @@
         <v>53</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E63" s="6" t="s">
         <v>93</v>
@@ -3027,7 +3036,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="64" spans="1:20" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A64" s="6" t="s">
         <v>52</v>
       </c>
@@ -3035,22 +3044,22 @@
         <v>53</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>144</v>
+        <v>93</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="G64" s="14" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A65" s="6" t="s">
         <v>52</v>
       </c>
@@ -3058,16 +3067,16 @@
         <v>53</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>93</v>
+        <v>144</v>
       </c>
       <c r="F65" s="6" t="s">
-        <v>117</v>
+        <v>145</v>
       </c>
       <c r="G65" s="14" t="s">
         <v>89</v>
@@ -3081,10 +3090,10 @@
         <v>53</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E66" s="6" t="s">
         <v>93</v>
@@ -3096,7 +3105,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A67" s="6" t="s">
         <v>52</v>
       </c>
@@ -3104,13 +3113,19 @@
         <v>53</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G67" s="15" t="s">
-        <v>25</v>
+        <v>111</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G67" s="14" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="21.6" x14ac:dyDescent="0.3">
@@ -3121,22 +3136,16 @@
         <v>53</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E68" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F68" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="G68" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+      <c r="G68" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A69" s="6" t="s">
         <v>52</v>
       </c>
@@ -3144,25 +3153,22 @@
         <v>53</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E69" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F69" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="G69" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="H69" s="7" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" ht="52.2" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F69" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G69" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A70" s="6" t="s">
         <v>52</v>
       </c>
@@ -3170,22 +3176,25 @@
         <v>53</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E70" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F70" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="G70" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+      <c r="E70" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F70" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G70" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="H70" s="7" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="52.2" x14ac:dyDescent="0.3">
       <c r="A71" s="6" t="s">
         <v>52</v>
       </c>
@@ -3193,10 +3202,10 @@
         <v>53</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>115</v>
+        <v>72</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>114</v>
       </c>
       <c r="E71" s="6" t="s">
         <v>93</v>
@@ -3216,16 +3225,22 @@
         <v>53</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="G72" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+      <c r="E72" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F72" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G72" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A73" s="6" t="s">
         <v>52</v>
       </c>
@@ -3233,22 +3248,16 @@
         <v>53</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="E73" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F73" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="G73" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+      <c r="G73" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="42" x14ac:dyDescent="0.3">
       <c r="A74" s="6" t="s">
         <v>52</v>
       </c>
@@ -3256,10 +3265,10 @@
         <v>53</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E74" s="6" t="s">
         <v>93</v>
@@ -3271,7 +3280,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A75" s="6" t="s">
         <v>52</v>
       </c>
@@ -3279,25 +3288,22 @@
         <v>53</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="E75" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F75" s="7" t="s">
-        <v>128</v>
+        <v>76</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E75" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F75" s="6" t="s">
+        <v>117</v>
       </c>
       <c r="G75" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="H75" s="7" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="76" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A76" s="6" t="s">
         <v>52</v>
       </c>
@@ -3305,19 +3311,22 @@
         <v>53</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="E76" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F76" s="6" t="s">
-        <v>117</v>
+        <v>77</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E76" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F76" s="7" t="s">
+        <v>128</v>
       </c>
       <c r="G76" s="14" t="s">
         <v>89</v>
+      </c>
+      <c r="H76" s="7" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="77" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
@@ -3328,10 +3337,10 @@
         <v>53</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E77" s="6" t="s">
         <v>93</v>
@@ -3351,16 +3360,16 @@
         <v>53</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="E78" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F78" s="7" t="s">
-        <v>128</v>
+        <v>121</v>
+      </c>
+      <c r="E78" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F78" s="6" t="s">
+        <v>117</v>
       </c>
       <c r="G78" s="14" t="s">
         <v>89</v>
@@ -3374,18 +3383,22 @@
         <v>53</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="E79" s="7"/>
-      <c r="F79" s="7"/>
-      <c r="G79" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" ht="21.6" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+      <c r="E79" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F79" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G79" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A80" s="6" t="s">
         <v>52</v>
       </c>
@@ -3393,22 +3406,18 @@
         <v>53</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="E80" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F80" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="G80" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+      <c r="E80" s="7"/>
+      <c r="F80" s="7"/>
+      <c r="G80" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A81" s="6" t="s">
         <v>52</v>
       </c>
@@ -3416,16 +3425,22 @@
         <v>53</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="G81" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+      <c r="E81" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F81" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G81" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A82" s="6" t="s">
         <v>52</v>
       </c>
@@ -3433,22 +3448,16 @@
         <v>53</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="E82" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F82" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="G82" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+      <c r="G82" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="42" x14ac:dyDescent="0.3">
       <c r="A83" s="6" t="s">
         <v>52</v>
       </c>
@@ -3456,13 +3465,19 @@
         <v>53</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>146</v>
+        <v>84</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="G83" s="15" t="s">
-        <v>25</v>
+        <v>126</v>
+      </c>
+      <c r="E83" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F83" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G83" s="14" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
@@ -3473,14 +3488,16 @@
         <v>53</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="D84" s="3"/>
+        <v>146</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>148</v>
+      </c>
       <c r="G84" s="15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="6" t="s">
         <v>52</v>
       </c>
@@ -3488,48 +3505,39 @@
         <v>53</v>
       </c>
       <c r="C85" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="D85" s="3"/>
+      <c r="G85" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
+      <c r="A86" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C86" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="D85" s="3" t="s">
+      <c r="D86" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="E85" s="6" t="s">
+      <c r="E86" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="F85" s="6" t="s">
+      <c r="F86" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="G85" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A86" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="B86" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C86" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D86" s="5"/>
-      <c r="E86" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F86" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="G86" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="H86" s="7" t="s">
-        <v>138</v>
+      <c r="G86" s="14" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="87" spans="1:8" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A87" s="7" t="s">
-        <v>165</v>
+        <v>86</v>
       </c>
       <c r="B87" s="7" t="s">
         <v>53</v>
@@ -3551,8 +3559,32 @@
         <v>138</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C88" s="7"/>
+    <row r="88" spans="1:8" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A88" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D88" s="5"/>
+      <c r="E88" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F88" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="G88" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="H88" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C89" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3562,6 +3594,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100919AB8A12910594B8F4D80F4ACA7D0E7" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9c71394a73500791d9f4b659570ff6f6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a318c9bd-5828-4914-8ac9-a57d8c01df7a" xmlns:ns3="4da7f078-0f32-436f-b12a-21525bae5a0e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f0993cb8e7f28d1e7915cb051b812a71" ns2:_="" ns3:_="">
     <xsd:import namespace="a318c9bd-5828-4914-8ac9-a57d8c01df7a"/>
@@ -3738,22 +3785,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC4DE233-B05C-40D4-9E0D-B697BD35B3E3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B8261F5-E2C2-49F8-99F3-13EB69507EB7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56F0D49C-4924-48A7-977F-FB48DDC11B03}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3770,21 +3819,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B8261F5-E2C2-49F8-99F3-13EB69507EB7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC4DE233-B05C-40D4-9E0D-B697BD35B3E3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Edited line that should be Remove
</commit_message>
<xml_diff>
--- a/Meta/flagsMap_withDecisions.xlsx
+++ b/Meta/flagsMap_withDecisions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/coffman_christian_epa_gov/Documents/Profile/Documents/Projects/GL_Data/Meta/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/vitense_kelsey_epa_gov/Documents/GL_Data/Meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="440" documentId="13_ncr:4000b_{6437034B-B068-4CF2-9A04-9208A97A6BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2DD346F7-97AE-43BB-BD74-162FA987B8CD}"/>
+  <xr:revisionPtr revIDLastSave="446" documentId="13_ncr:4000b_{6437034B-B068-4CF2-9A04-9208A97A6BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F68F4C4-423C-49DA-B398-DA5A65B9575A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="flagsMap_withDecisions" sheetId="1" r:id="rId1"/>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="173">
   <si>
     <t>Study</t>
   </si>
@@ -588,9 +588,6 @@
     <t>MDL imputed</t>
   </si>
   <si>
-    <t>Christian Filled these in. Needs verification</t>
-  </si>
-  <si>
     <t>CSMI_2021</t>
   </si>
   <si>
@@ -615,7 +612,7 @@
     <t>T</t>
   </si>
   <si>
-    <t>time issue</t>
+    <t>Time imputed</t>
   </si>
 </sst>
 </file>
@@ -769,7 +766,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="38">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -973,12 +970,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1140,7 +1131,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1184,9 +1175,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1586,24 +1574,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="44.33203125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="38.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.3125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5234375" style="6" customWidth="1"/>
+    <col min="3" max="3" width="44.3125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="38.5234375" style="1" customWidth="1"/>
     <col min="5" max="5" width="15" style="6" customWidth="1"/>
     <col min="6" max="6" width="26" style="6" customWidth="1"/>
-    <col min="7" max="7" width="10.5546875" style="6" customWidth="1"/>
-    <col min="8" max="8" width="35.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="6"/>
+    <col min="7" max="7" width="10.5234375" style="6" customWidth="1"/>
+    <col min="8" max="8" width="35.1015625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.89453125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1629,24 +1617,24 @@
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>30</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G2" s="13" t="s">
         <v>132</v>
@@ -1655,24 +1643,24 @@
         <v>138</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="7" t="s">
         <v>86</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>30</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G3" s="13" t="s">
         <v>132</v>
@@ -1681,24 +1669,24 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="6" t="s">
         <v>52</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>30</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G4" s="13" t="s">
         <v>132</v>
@@ -1707,24 +1695,24 @@
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="10" t="s">
         <v>50</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>30</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G5" s="13" t="s">
         <v>132</v>
@@ -1733,24 +1721,24 @@
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>30</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G6" s="13" t="s">
         <v>132</v>
@@ -1759,24 +1747,24 @@
         <v>138</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>30</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G7" s="13" t="s">
         <v>132</v>
@@ -1785,24 +1773,24 @@
         <v>138</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>30</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G8" s="13" t="s">
         <v>132</v>
@@ -1811,24 +1799,24 @@
         <v>138</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>30</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G9" s="13" t="s">
         <v>132</v>
@@ -1837,24 +1825,24 @@
         <v>138</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>30</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G10" s="13" t="s">
         <v>132</v>
@@ -1863,7 +1851,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="6" t="s">
         <v>4</v>
       </c>
@@ -1877,14 +1865,11 @@
         <v>19</v>
       </c>
       <c r="F11" s="7"/>
-      <c r="G11" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G11" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="6" t="s">
         <v>4</v>
       </c>
@@ -1905,7 +1890,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="6" t="s">
         <v>4</v>
       </c>
@@ -1928,7 +1913,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="6" t="s">
         <v>4</v>
       </c>
@@ -1954,7 +1939,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="6" t="s">
         <v>4</v>
       </c>
@@ -1974,7 +1959,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="6" t="s">
         <v>4</v>
       </c>
@@ -1994,7 +1979,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="6" t="s">
         <v>4</v>
       </c>
@@ -2012,7 +1997,7 @@
       </c>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="6" t="s">
         <v>4</v>
       </c>
@@ -2030,7 +2015,7 @@
       </c>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="6" t="s">
         <v>4</v>
       </c>
@@ -2048,7 +2033,7 @@
       </c>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="6" t="s">
         <v>4</v>
       </c>
@@ -2061,11 +2046,9 @@
       <c r="G20" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="H20" s="17" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H20" s="11"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="6" t="s">
         <v>4</v>
       </c>
@@ -2078,11 +2061,9 @@
       <c r="G21" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="H21" s="17" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="H21" s="11"/>
+    </row>
+    <row r="22" spans="1:8" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="6" t="s">
         <v>4</v>
       </c>
@@ -2099,7 +2080,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="6" t="s">
         <v>4</v>
       </c>
@@ -2116,7 +2097,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="6" t="s">
         <v>4</v>
       </c>
@@ -2133,7 +2114,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="6" t="s">
         <v>4</v>
       </c>
@@ -2150,7 +2131,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="6" t="s">
         <v>4</v>
       </c>
@@ -2170,7 +2151,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="7" t="s">
         <v>4</v>
       </c>
@@ -2193,7 +2174,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="7" t="s">
         <v>4</v>
       </c>
@@ -2216,7 +2197,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="6" t="s">
         <v>23</v>
       </c>
@@ -2227,7 +2208,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="6" t="s">
         <v>23</v>
       </c>
@@ -2238,7 +2219,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="6" t="s">
         <v>23</v>
       </c>
@@ -2264,7 +2245,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="6" t="s">
         <v>27</v>
       </c>
@@ -2290,7 +2271,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="6" t="s">
         <v>27</v>
       </c>
@@ -2313,7 +2294,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="6" t="s">
         <v>29</v>
       </c>
@@ -2330,7 +2311,7 @@
         <v>30</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G34" s="13" t="s">
         <v>132</v>
@@ -2339,7 +2320,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="6" t="s">
         <v>29</v>
       </c>
@@ -2363,7 +2344,7 @@
       </c>
       <c r="H35" s="7"/>
     </row>
-    <row r="36" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="6" t="s">
         <v>29</v>
       </c>
@@ -2380,7 +2361,7 @@
         <v>30</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G36" s="13" t="s">
         <v>132</v>
@@ -2389,7 +2370,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="6" t="s">
         <v>29</v>
       </c>
@@ -2412,7 +2393,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="6" t="s">
         <v>29</v>
       </c>
@@ -2432,7 +2413,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="6" t="s">
         <v>29</v>
       </c>
@@ -2455,7 +2436,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="6" t="s">
         <v>29</v>
       </c>
@@ -2469,7 +2450,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="6" t="s">
         <v>29</v>
       </c>
@@ -2489,7 +2470,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="6" t="s">
         <v>29</v>
       </c>
@@ -2509,7 +2490,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="1:20" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="10" t="s">
         <v>50</v>
       </c>
@@ -2521,7 +2502,7 @@
       </c>
       <c r="D43" s="9"/>
       <c r="E43" s="10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F43" s="10" t="s">
         <v>154</v>
@@ -2533,7 +2514,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="44" spans="1:20" s="10" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="7" t="s">
         <v>50</v>
       </c>
@@ -2548,7 +2529,7 @@
         <v>30</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G44" s="13" t="s">
         <v>132</v>
@@ -2569,7 +2550,7 @@
       <c r="S44" s="7"/>
       <c r="T44" s="7"/>
     </row>
-    <row r="45" spans="1:20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
         <v>50</v>
       </c>
@@ -2592,7 +2573,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="46" spans="1:20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:20" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
         <v>50</v>
       </c>
@@ -2615,7 +2596,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
         <v>50</v>
       </c>
@@ -2638,7 +2619,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="48" spans="1:20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
         <v>50</v>
       </c>
@@ -2661,7 +2642,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="49" spans="1:20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
         <v>50</v>
       </c>
@@ -2684,7 +2665,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="50" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="7" t="s">
         <v>50</v>
       </c>
@@ -2718,7 +2699,7 @@
       <c r="S50" s="7"/>
       <c r="T50" s="7"/>
     </row>
-    <row r="51" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="7" t="s">
         <v>50</v>
       </c>
@@ -2752,7 +2733,7 @@
       <c r="S51" s="7"/>
       <c r="T51" s="7"/>
     </row>
-    <row r="52" spans="1:20" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20" ht="21.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="6" t="s">
         <v>52</v>
       </c>
@@ -2760,23 +2741,23 @@
         <v>53</v>
       </c>
       <c r="C52" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="D52" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="E52" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="E52" s="6" t="s">
+      <c r="F52" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="F52" s="6" t="s">
-        <v>173</v>
-      </c>
       <c r="G52" s="14" t="s">
         <v>89</v>
       </c>
       <c r="H52" s="7"/>
     </row>
-    <row r="53" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:20" ht="31.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="6" t="s">
         <v>52</v>
       </c>
@@ -2800,7 +2781,7 @@
       </c>
       <c r="H53" s="7"/>
     </row>
-    <row r="54" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:20" ht="31.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="6" t="s">
         <v>52</v>
       </c>
@@ -2823,7 +2804,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:20" ht="31.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="6" t="s">
         <v>52</v>
       </c>
@@ -2846,7 +2827,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:20" ht="31.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="6" t="s">
         <v>52</v>
       </c>
@@ -2869,7 +2850,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:20" ht="31.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="6" t="s">
         <v>52</v>
       </c>
@@ -2892,7 +2873,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:20" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="6" t="s">
         <v>52</v>
       </c>
@@ -2909,7 +2890,7 @@
         <v>30</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G58" s="13" t="s">
         <v>132</v>
@@ -2918,7 +2899,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:20" ht="31.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="6" t="s">
         <v>52</v>
       </c>
@@ -2941,7 +2922,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:20" ht="31.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="6" t="s">
         <v>52</v>
       </c>
@@ -2964,7 +2945,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="61" spans="1:20" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:20" ht="21.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="6" t="s">
         <v>52</v>
       </c>
@@ -2987,7 +2968,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="62" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:20" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="6" t="s">
         <v>52</v>
       </c>
@@ -3004,7 +2985,7 @@
         <v>30</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G62" s="13" t="s">
         <v>132</v>
@@ -3013,7 +2994,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="63" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:20" ht="31.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="6" t="s">
         <v>52</v>
       </c>
@@ -3036,7 +3017,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="64" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:20" ht="31.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="6" t="s">
         <v>52</v>
       </c>
@@ -3059,7 +3040,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" ht="21.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="6" t="s">
         <v>52</v>
       </c>
@@ -3082,7 +3063,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" ht="31.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="6" t="s">
         <v>52</v>
       </c>
@@ -3105,7 +3086,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" ht="31.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="6" t="s">
         <v>52</v>
       </c>
@@ -3128,7 +3109,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" ht="21.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="6" t="s">
         <v>52</v>
       </c>
@@ -3145,7 +3126,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" ht="21.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="6" t="s">
         <v>52</v>
       </c>
@@ -3168,7 +3149,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="6" t="s">
         <v>52</v>
       </c>
@@ -3194,7 +3175,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="52.2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" ht="52.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="6" t="s">
         <v>52</v>
       </c>
@@ -3217,7 +3198,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" ht="31.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" s="6" t="s">
         <v>52</v>
       </c>
@@ -3240,7 +3221,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" ht="31.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" s="6" t="s">
         <v>52</v>
       </c>
@@ -3257,7 +3238,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" ht="42" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" s="6" t="s">
         <v>52</v>
       </c>
@@ -3280,7 +3261,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" ht="31.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" s="6" t="s">
         <v>52</v>
       </c>
@@ -3303,7 +3284,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" s="6" t="s">
         <v>52</v>
       </c>
@@ -3329,7 +3310,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" ht="31.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" s="6" t="s">
         <v>52</v>
       </c>
@@ -3352,7 +3333,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" ht="31.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" s="6" t="s">
         <v>52</v>
       </c>
@@ -3375,7 +3356,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" ht="31.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="6" t="s">
         <v>52</v>
       </c>
@@ -3398,7 +3379,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" ht="31.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="6" t="s">
         <v>52</v>
       </c>
@@ -3417,7 +3398,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" ht="21.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="6" t="s">
         <v>52</v>
       </c>
@@ -3440,7 +3421,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" ht="31.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="6" t="s">
         <v>52</v>
       </c>
@@ -3457,7 +3438,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" ht="42" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="6" t="s">
         <v>52</v>
       </c>
@@ -3480,7 +3461,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="6" t="s">
         <v>52</v>
       </c>
@@ -3497,7 +3478,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="6" t="s">
         <v>52</v>
       </c>
@@ -3512,7 +3493,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" ht="31.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="6" t="s">
         <v>52</v>
       </c>
@@ -3535,7 +3516,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="87" spans="1:8" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="7" t="s">
         <v>86</v>
       </c>
@@ -3550,7 +3531,7 @@
         <v>30</v>
       </c>
       <c r="F87" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G87" s="13" t="s">
         <v>132</v>
@@ -3559,9 +3540,9 @@
         <v>138</v>
       </c>
     </row>
-    <row r="88" spans="1:8" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B88" s="7" t="s">
         <v>53</v>
@@ -3574,7 +3555,7 @@
         <v>30</v>
       </c>
       <c r="F88" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G88" s="13" t="s">
         <v>132</v>
@@ -3583,7 +3564,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C89" s="7"/>
     </row>
   </sheetData>
@@ -3594,21 +3575,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100919AB8A12910594B8F4D80F4ACA7D0E7" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9c71394a73500791d9f4b659570ff6f6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a318c9bd-5828-4914-8ac9-a57d8c01df7a" xmlns:ns3="4da7f078-0f32-436f-b12a-21525bae5a0e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f0993cb8e7f28d1e7915cb051b812a71" ns2:_="" ns3:_="">
     <xsd:import namespace="a318c9bd-5828-4914-8ac9-a57d8c01df7a"/>
@@ -3785,24 +3751,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC4DE233-B05C-40D4-9E0D-B697BD35B3E3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B8261F5-E2C2-49F8-99F3-13EB69507EB7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56F0D49C-4924-48A7-977F-FB48DDC11B03}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3819,4 +3783,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B8261F5-E2C2-49F8-99F3-13EB69507EB7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC4DE233-B05C-40D4-9E0D-B697BD35B3E3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Edited hydro2015 QA actions to keep all
</commit_message>
<xml_diff>
--- a/Meta/flagsMap_withDecisions.xlsx
+++ b/Meta/flagsMap_withDecisions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/vitense_kelsey_epa_gov/Documents/GL_Data/Meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="446" documentId="13_ncr:4000b_{6437034B-B068-4CF2-9A04-9208A97A6BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F68F4C4-423C-49DA-B398-DA5A65B9575A}"/>
+  <xr:revisionPtr revIDLastSave="450" documentId="13_ncr:4000b_{6437034B-B068-4CF2-9A04-9208A97A6BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6C55357-A902-46A1-86FE-0BF6BBCB1D53}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-57720" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="flagsMap_withDecisions" sheetId="1" r:id="rId1"/>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="175">
   <si>
     <t>Study</t>
   </si>
@@ -613,6 +613,12 @@
   </si>
   <si>
     <t>Time imputed</t>
+  </si>
+  <si>
+    <t>Should be removed anyway because all NA</t>
+  </si>
+  <si>
+    <t>only catches one case of where UW &gt; AMB light. There are other similar cases as well, so don't remove these.</t>
   </si>
 </sst>
 </file>
@@ -1242,9 +1248,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1282,7 +1288,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1388,7 +1394,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1530,7 +1536,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1574,24 +1580,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.3125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5234375" style="6" customWidth="1"/>
-    <col min="3" max="3" width="44.3125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="38.5234375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="44.33203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="38.5546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="15" style="6" customWidth="1"/>
     <col min="6" max="6" width="26" style="6" customWidth="1"/>
-    <col min="7" max="7" width="10.5234375" style="6" customWidth="1"/>
-    <col min="8" max="8" width="35.1015625" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.89453125" style="6"/>
+    <col min="7" max="7" width="10.5546875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="35.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1617,7 +1623,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>164</v>
       </c>
@@ -1643,7 +1649,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>86</v>
       </c>
@@ -1669,7 +1675,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>52</v>
       </c>
@@ -1695,7 +1701,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>50</v>
       </c>
@@ -1721,7 +1727,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>29</v>
       </c>
@@ -1747,7 +1753,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>27</v>
       </c>
@@ -1773,7 +1779,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>23</v>
       </c>
@@ -1799,7 +1805,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
@@ -1825,7 +1831,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>4</v>
       </c>
@@ -1851,7 +1857,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>4</v>
       </c>
@@ -1869,7 +1875,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>4</v>
       </c>
@@ -1890,7 +1896,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>4</v>
       </c>
@@ -1913,7 +1919,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>4</v>
       </c>
@@ -1939,7 +1945,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>4</v>
       </c>
@@ -1959,7 +1965,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>4</v>
       </c>
@@ -1979,7 +1985,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>4</v>
       </c>
@@ -1997,7 +2003,7 @@
       </c>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>4</v>
       </c>
@@ -2015,7 +2021,7 @@
       </c>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>4</v>
       </c>
@@ -2033,7 +2039,7 @@
       </c>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>4</v>
       </c>
@@ -2048,7 +2054,7 @@
       </c>
       <c r="H20" s="11"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>4</v>
       </c>
@@ -2063,7 +2069,7 @@
       </c>
       <c r="H21" s="11"/>
     </row>
-    <row r="22" spans="1:8" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>4</v>
       </c>
@@ -2080,7 +2086,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>4</v>
       </c>
@@ -2097,7 +2103,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>4</v>
       </c>
@@ -2114,7 +2120,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>4</v>
       </c>
@@ -2131,7 +2137,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>4</v>
       </c>
@@ -2151,7 +2157,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
         <v>4</v>
       </c>
@@ -2174,7 +2180,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
         <v>4</v>
       </c>
@@ -2197,29 +2203,35 @@
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G29" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="G29" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G30" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="G30" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>23</v>
       </c>
@@ -2245,7 +2257,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>27</v>
       </c>
@@ -2271,7 +2283,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
         <v>27</v>
       </c>
@@ -2294,7 +2306,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
         <v>29</v>
       </c>
@@ -2320,7 +2332,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
         <v>29</v>
       </c>
@@ -2344,7 +2356,7 @@
       </c>
       <c r="H35" s="7"/>
     </row>
-    <row r="36" spans="1:20" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
         <v>29</v>
       </c>
@@ -2370,7 +2382,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
         <v>29</v>
       </c>
@@ -2393,7 +2405,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
         <v>29</v>
       </c>
@@ -2413,7 +2425,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
         <v>29</v>
       </c>
@@ -2436,7 +2448,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
         <v>29</v>
       </c>
@@ -2450,7 +2462,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>29</v>
       </c>
@@ -2470,7 +2482,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
         <v>29</v>
       </c>
@@ -2490,7 +2502,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="1:20" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:20" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A43" s="10" t="s">
         <v>50</v>
       </c>
@@ -2514,7 +2526,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="44" spans="1:20" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:20" s="10" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>50</v>
       </c>
@@ -2550,7 +2562,7 @@
       <c r="S44" s="7"/>
       <c r="T44" s="7"/>
     </row>
-    <row r="45" spans="1:20" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>50</v>
       </c>
@@ -2573,7 +2585,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="46" spans="1:20" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>50</v>
       </c>
@@ -2596,7 +2608,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:20" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>50</v>
       </c>
@@ -2619,7 +2631,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="48" spans="1:20" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>50</v>
       </c>
@@ -2642,7 +2654,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="49" spans="1:20" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:20" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>50</v>
       </c>
@@ -2665,7 +2677,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="50" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
         <v>50</v>
       </c>
@@ -2699,7 +2711,7 @@
       <c r="S50" s="7"/>
       <c r="T50" s="7"/>
     </row>
-    <row r="51" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
         <v>50</v>
       </c>
@@ -2733,7 +2745,7 @@
       <c r="S51" s="7"/>
       <c r="T51" s="7"/>
     </row>
-    <row r="52" spans="1:20" ht="21.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:20" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A52" s="6" t="s">
         <v>52</v>
       </c>
@@ -2757,7 +2769,7 @@
       </c>
       <c r="H52" s="7"/>
     </row>
-    <row r="53" spans="1:20" ht="31.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A53" s="6" t="s">
         <v>52</v>
       </c>
@@ -2781,7 +2793,7 @@
       </c>
       <c r="H53" s="7"/>
     </row>
-    <row r="54" spans="1:20" ht="31.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
         <v>52</v>
       </c>
@@ -2804,7 +2816,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="31.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
         <v>52</v>
       </c>
@@ -2827,7 +2839,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="31.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A56" s="6" t="s">
         <v>52</v>
       </c>
@@ -2850,7 +2862,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="31.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A57" s="6" t="s">
         <v>52</v>
       </c>
@@ -2873,7 +2885,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="129.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:20" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A58" s="6" t="s">
         <v>52</v>
       </c>
@@ -2899,7 +2911,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="31.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A59" s="6" t="s">
         <v>52</v>
       </c>
@@ -2922,7 +2934,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="31.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A60" s="6" t="s">
         <v>52</v>
       </c>
@@ -2945,7 +2957,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="61" spans="1:20" ht="21.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:20" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A61" s="6" t="s">
         <v>52</v>
       </c>
@@ -2968,7 +2980,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="62" spans="1:20" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A62" s="6" t="s">
         <v>52</v>
       </c>
@@ -2994,7 +3006,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="63" spans="1:20" ht="31.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A63" s="6" t="s">
         <v>52</v>
       </c>
@@ -3017,7 +3029,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="64" spans="1:20" ht="31.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A64" s="6" t="s">
         <v>52</v>
       </c>
@@ -3040,7 +3052,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="21.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:8" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A65" s="6" t="s">
         <v>52</v>
       </c>
@@ -3063,7 +3075,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="31.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A66" s="6" t="s">
         <v>52</v>
       </c>
@@ -3086,7 +3098,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="31.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A67" s="6" t="s">
         <v>52</v>
       </c>
@@ -3109,7 +3121,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="21.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:8" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A68" s="6" t="s">
         <v>52</v>
       </c>
@@ -3126,7 +3138,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="21.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:8" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A69" s="6" t="s">
         <v>52</v>
       </c>
@@ -3149,7 +3161,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A70" s="6" t="s">
         <v>52</v>
       </c>
@@ -3175,7 +3187,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="52.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:8" ht="52.2" x14ac:dyDescent="0.3">
       <c r="A71" s="6" t="s">
         <v>52</v>
       </c>
@@ -3198,7 +3210,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="31.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A72" s="6" t="s">
         <v>52</v>
       </c>
@@ -3221,7 +3233,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="31.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A73" s="6" t="s">
         <v>52</v>
       </c>
@@ -3238,7 +3250,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="42" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:8" ht="42" x14ac:dyDescent="0.3">
       <c r="A74" s="6" t="s">
         <v>52</v>
       </c>
@@ -3261,7 +3273,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="31.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A75" s="6" t="s">
         <v>52</v>
       </c>
@@ -3284,7 +3296,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A76" s="6" t="s">
         <v>52</v>
       </c>
@@ -3310,7 +3322,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="31.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A77" s="6" t="s">
         <v>52</v>
       </c>
@@ -3333,7 +3345,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="31.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A78" s="6" t="s">
         <v>52</v>
       </c>
@@ -3356,7 +3368,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="31.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A79" s="6" t="s">
         <v>52</v>
       </c>
@@ -3379,7 +3391,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="31.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A80" s="6" t="s">
         <v>52</v>
       </c>
@@ -3398,7 +3410,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="21.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:8" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A81" s="6" t="s">
         <v>52</v>
       </c>
@@ -3421,7 +3433,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="31.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A82" s="6" t="s">
         <v>52</v>
       </c>
@@ -3438,7 +3450,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="42" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:8" ht="42" x14ac:dyDescent="0.3">
       <c r="A83" s="6" t="s">
         <v>52</v>
       </c>
@@ -3461,7 +3473,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="6" t="s">
         <v>52</v>
       </c>
@@ -3478,7 +3490,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="6" t="s">
         <v>52</v>
       </c>
@@ -3493,7 +3505,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="31.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A86" s="6" t="s">
         <v>52</v>
       </c>
@@ -3516,7 +3528,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="87" spans="1:8" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:8" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A87" s="7" t="s">
         <v>86</v>
       </c>
@@ -3540,7 +3552,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="88" spans="1:8" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:8" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A88" s="7" t="s">
         <v>164</v>
       </c>
@@ -3564,7 +3576,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C89" s="7"/>
     </row>
   </sheetData>
@@ -3575,6 +3587,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100919AB8A12910594B8F4D80F4ACA7D0E7" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9c71394a73500791d9f4b659570ff6f6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a318c9bd-5828-4914-8ac9-a57d8c01df7a" xmlns:ns3="4da7f078-0f32-436f-b12a-21525bae5a0e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f0993cb8e7f28d1e7915cb051b812a71" ns2:_="" ns3:_="">
     <xsd:import namespace="a318c9bd-5828-4914-8ac9-a57d8c01df7a"/>
@@ -3751,22 +3778,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC4DE233-B05C-40D4-9E0D-B697BD35B3E3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B8261F5-E2C2-49F8-99F3-13EB69507EB7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56F0D49C-4924-48A7-977F-FB48DDC11B03}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3783,21 +3812,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B8261F5-E2C2-49F8-99F3-13EB69507EB7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC4DE233-B05C-40D4-9E0D-B697BD35B3E3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added time and secchi CTB flags for NOAA
</commit_message>
<xml_diff>
--- a/Meta/flagsMap_withDecisions.xlsx
+++ b/Meta/flagsMap_withDecisions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/vitense_kelsey_epa_gov/Documents/GL_Data/Meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="450" documentId="13_ncr:4000b_{6437034B-B068-4CF2-9A04-9208A97A6BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6C55357-A902-46A1-86FE-0BF6BBCB1D53}"/>
+  <xr:revisionPtr revIDLastSave="461" documentId="13_ncr:4000b_{6437034B-B068-4CF2-9A04-9208A97A6BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12D9D468-7F45-425A-9914-E4483D48E857}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-61548" yWindow="-1872" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="flagsMap_withDecisions" sheetId="1" r:id="rId1"/>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="177">
   <si>
     <t>Study</t>
   </si>
@@ -619,6 +619,12 @@
   </si>
   <si>
     <t>only catches one case of where UW &gt; AMB light. There are other similar cases as well, so don't remove these.</t>
+  </si>
+  <si>
+    <t>NOAA_WQ</t>
+  </si>
+  <si>
+    <t>time imputed as noon</t>
   </si>
 </sst>
 </file>
@@ -1578,26 +1584,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T89"/>
+  <dimension ref="A1:T90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="44.33203125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="38.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="44.28515625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="38.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="15" style="6" customWidth="1"/>
     <col min="6" max="6" width="26" style="6" customWidth="1"/>
-    <col min="7" max="7" width="10.5546875" style="6" customWidth="1"/>
-    <col min="8" max="8" width="35.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="6"/>
+    <col min="7" max="7" width="10.5703125" style="6" customWidth="1"/>
+    <col min="8" max="8" width="35.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1623,7 +1629,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>164</v>
       </c>
@@ -1649,7 +1655,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>86</v>
       </c>
@@ -1675,7 +1681,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>52</v>
       </c>
@@ -1701,7 +1707,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>50</v>
       </c>
@@ -1727,7 +1733,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>29</v>
       </c>
@@ -1753,7 +1759,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>27</v>
       </c>
@@ -1779,7 +1785,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>23</v>
       </c>
@@ -1805,7 +1811,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
@@ -1831,7 +1837,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>4</v>
       </c>
@@ -1857,7 +1863,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>4</v>
       </c>
@@ -1875,7 +1881,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>4</v>
       </c>
@@ -1896,7 +1902,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>4</v>
       </c>
@@ -1919,7 +1925,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>4</v>
       </c>
@@ -1945,7 +1951,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>4</v>
       </c>
@@ -1965,7 +1971,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>4</v>
       </c>
@@ -1985,7 +1991,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>4</v>
       </c>
@@ -2003,7 +2009,7 @@
       </c>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>4</v>
       </c>
@@ -2021,7 +2027,7 @@
       </c>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>4</v>
       </c>
@@ -2039,7 +2045,7 @@
       </c>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>4</v>
       </c>
@@ -2054,7 +2060,7 @@
       </c>
       <c r="H20" s="11"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>4</v>
       </c>
@@ -2069,7 +2075,7 @@
       </c>
       <c r="H21" s="11"/>
     </row>
-    <row r="22" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>4</v>
       </c>
@@ -2086,7 +2092,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>4</v>
       </c>
@@ -2103,7 +2109,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>4</v>
       </c>
@@ -2120,7 +2126,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>4</v>
       </c>
@@ -2137,7 +2143,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>4</v>
       </c>
@@ -2157,7 +2163,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>4</v>
       </c>
@@ -2180,7 +2186,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>4</v>
       </c>
@@ -2203,7 +2209,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>23</v>
       </c>
@@ -2217,7 +2223,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>23</v>
       </c>
@@ -2231,7 +2237,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>23</v>
       </c>
@@ -2257,7 +2263,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>27</v>
       </c>
@@ -2283,7 +2289,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>27</v>
       </c>
@@ -2306,7 +2312,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>29</v>
       </c>
@@ -2332,7 +2338,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>29</v>
       </c>
@@ -2356,7 +2362,7 @@
       </c>
       <c r="H35" s="7"/>
     </row>
-    <row r="36" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>29</v>
       </c>
@@ -2382,7 +2388,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>29</v>
       </c>
@@ -2405,7 +2411,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>29</v>
       </c>
@@ -2425,7 +2431,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>29</v>
       </c>
@@ -2448,7 +2454,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>29</v>
       </c>
@@ -2462,7 +2468,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>29</v>
       </c>
@@ -2482,7 +2488,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>29</v>
       </c>
@@ -2502,7 +2508,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="1:20" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
         <v>50</v>
       </c>
@@ -2526,7 +2532,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="44" spans="1:20" s="10" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>50</v>
       </c>
@@ -2562,7 +2568,7 @@
       <c r="S44" s="7"/>
       <c r="T44" s="7"/>
     </row>
-    <row r="45" spans="1:20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>50</v>
       </c>
@@ -2585,7 +2591,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="46" spans="1:20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>50</v>
       </c>
@@ -2608,7 +2614,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>50</v>
       </c>
@@ -2631,7 +2637,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="48" spans="1:20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>50</v>
       </c>
@@ -2654,7 +2660,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="49" spans="1:20" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>50</v>
       </c>
@@ -2677,7 +2683,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="50" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:20" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>50</v>
       </c>
@@ -2711,7 +2717,7 @@
       <c r="S50" s="7"/>
       <c r="T50" s="7"/>
     </row>
-    <row r="51" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:20" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>50</v>
       </c>
@@ -2745,7 +2751,7 @@
       <c r="S51" s="7"/>
       <c r="T51" s="7"/>
     </row>
-    <row r="52" spans="1:20" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>52</v>
       </c>
@@ -2753,23 +2759,23 @@
         <v>53</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>169</v>
+        <v>54</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>170</v>
+        <v>99</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>171</v>
+        <v>93</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>172</v>
+        <v>117</v>
       </c>
       <c r="G52" s="14" t="s">
         <v>89</v>
       </c>
       <c r="H52" s="7"/>
     </row>
-    <row r="53" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:20" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>52</v>
       </c>
@@ -2777,10 +2783,10 @@
         <v>53</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E53" s="6" t="s">
         <v>93</v>
@@ -2791,9 +2797,8 @@
       <c r="G53" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="H53" s="7"/>
-    </row>
-    <row r="54" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:20" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>52</v>
       </c>
@@ -2801,22 +2806,22 @@
         <v>53</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F54" s="6" t="s">
-        <v>117</v>
+        <v>92</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="G54" s="14" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:20" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
         <v>52</v>
       </c>
@@ -2824,22 +2829,22 @@
         <v>53</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>41</v>
+        <v>93</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>117</v>
       </c>
       <c r="G55" s="14" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:20" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>52</v>
       </c>
@@ -2847,10 +2852,10 @@
         <v>53</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E56" s="6" t="s">
         <v>93</v>
@@ -2862,7 +2867,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:20" ht="165" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
         <v>52</v>
       </c>
@@ -2870,22 +2875,25 @@
         <v>53</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="E57" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F57" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="G57" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="58" spans="1:20" ht="129.6" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G57" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="H57" s="7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
         <v>52</v>
       </c>
@@ -2893,25 +2901,22 @@
         <v>53</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>30</v>
+        <v>93</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="G58" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="H58" s="7" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="59" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+      <c r="G58" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
         <v>52</v>
       </c>
@@ -2919,10 +2924,10 @@
         <v>53</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E59" s="7" t="s">
         <v>93</v>
@@ -2934,7 +2939,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:20" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
         <v>52</v>
       </c>
@@ -2942,22 +2947,22 @@
         <v>53</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="G60" s="14" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="61" spans="1:20" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:20" ht="60" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
         <v>52</v>
       </c>
@@ -2965,22 +2970,25 @@
         <v>53</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="E61" s="7" t="s">
-        <v>94</v>
+        <v>30</v>
       </c>
       <c r="F61" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="G61" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="62" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
+        <v>166</v>
+      </c>
+      <c r="G61" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="H61" s="7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
         <v>52</v>
       </c>
@@ -2988,25 +2996,22 @@
         <v>53</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E62" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F62" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="G62" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="H62" s="7" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="63" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G62" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
         <v>52</v>
       </c>
@@ -3014,10 +3019,10 @@
         <v>53</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E63" s="6" t="s">
         <v>93</v>
@@ -3029,7 +3034,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="64" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:20" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
         <v>52</v>
       </c>
@@ -3037,22 +3042,22 @@
         <v>53</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>93</v>
+        <v>144</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>117</v>
+        <v>145</v>
       </c>
       <c r="G64" s="14" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
         <v>52</v>
       </c>
@@ -3060,22 +3065,22 @@
         <v>53</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>144</v>
+        <v>93</v>
       </c>
       <c r="F65" s="6" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="G65" s="14" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
         <v>52</v>
       </c>
@@ -3083,10 +3088,10 @@
         <v>53</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E66" s="6" t="s">
         <v>93</v>
@@ -3098,7 +3103,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>52</v>
       </c>
@@ -3106,22 +3111,16 @@
         <v>53</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E67" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F67" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="G67" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" ht="21.6" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+      <c r="G67" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
         <v>52</v>
       </c>
@@ -3129,16 +3128,22 @@
         <v>53</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G68" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" ht="21.6" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G68" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
         <v>52</v>
       </c>
@@ -3146,22 +3151,25 @@
         <v>53</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E69" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F69" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="G69" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+      <c r="E69" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F69" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G69" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="H69" s="7" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
         <v>52</v>
       </c>
@@ -3169,25 +3177,22 @@
         <v>53</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E70" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F70" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="G70" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="H70" s="7" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" ht="52.2" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F70" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G70" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
         <v>52</v>
       </c>
@@ -3195,10 +3200,10 @@
         <v>53</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>114</v>
+        <v>73</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="E71" s="6" t="s">
         <v>93</v>
@@ -3210,7 +3215,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
         <v>52</v>
       </c>
@@ -3218,22 +3223,16 @@
         <v>53</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="E72" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F72" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="G72" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+      <c r="G72" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="57" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
         <v>52</v>
       </c>
@@ -3241,16 +3240,22 @@
         <v>53</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="G73" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+      <c r="E73" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F73" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G73" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
         <v>52</v>
       </c>
@@ -3258,10 +3263,10 @@
         <v>53</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E74" s="6" t="s">
         <v>93</v>
@@ -3273,7 +3278,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
         <v>52</v>
       </c>
@@ -3281,22 +3286,25 @@
         <v>53</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D75" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E75" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F75" s="6" t="s">
-        <v>117</v>
+        <v>77</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E75" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F75" s="7" t="s">
+        <v>128</v>
       </c>
       <c r="G75" s="14" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="H75" s="7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
         <v>52</v>
       </c>
@@ -3304,25 +3312,22 @@
         <v>53</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="E76" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F76" s="7" t="s">
-        <v>128</v>
+        <v>78</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E76" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F76" s="6" t="s">
+        <v>117</v>
       </c>
       <c r="G76" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="H76" s="7" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="77" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
         <v>52</v>
       </c>
@@ -3330,10 +3335,10 @@
         <v>53</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E77" s="6" t="s">
         <v>93</v>
@@ -3345,7 +3350,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
         <v>52</v>
       </c>
@@ -3353,22 +3358,22 @@
         <v>53</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="E78" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F78" s="6" t="s">
-        <v>117</v>
+        <v>122</v>
+      </c>
+      <c r="E78" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F78" s="7" t="s">
+        <v>128</v>
       </c>
       <c r="G78" s="14" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
         <v>52</v>
       </c>
@@ -3376,22 +3381,18 @@
         <v>53</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="E79" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F79" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="G79" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+      <c r="E79" s="7"/>
+      <c r="F79" s="7"/>
+      <c r="G79" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
         <v>52</v>
       </c>
@@ -3399,18 +3400,22 @@
         <v>53</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="E80" s="7"/>
-      <c r="F80" s="7"/>
-      <c r="G80" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" ht="21.6" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+      <c r="E80" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F80" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G80" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
         <v>52</v>
       </c>
@@ -3418,22 +3423,16 @@
         <v>53</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="E81" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F81" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="G81" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+      <c r="G81" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
         <v>52</v>
       </c>
@@ -3441,16 +3440,22 @@
         <v>53</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="G82" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+      <c r="E82" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F82" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G82" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
         <v>52</v>
       </c>
@@ -3458,22 +3463,16 @@
         <v>53</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>84</v>
+        <v>146</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="E83" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F83" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="G83" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+      <c r="G83" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
         <v>52</v>
       </c>
@@ -3481,16 +3480,14 @@
         <v>53</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="D84" s="3" t="s">
-        <v>148</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="D84" s="3"/>
       <c r="G84" s="15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
         <v>52</v>
       </c>
@@ -3498,14 +3495,22 @@
         <v>53</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="D85" s="3"/>
-      <c r="G85" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E85" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F85" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G85" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
         <v>52</v>
       </c>
@@ -3513,22 +3518,23 @@
         <v>53</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D86" s="3" t="s">
-        <v>127</v>
+        <v>169</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="E86" s="6" t="s">
-        <v>93</v>
+        <v>171</v>
       </c>
       <c r="F86" s="6" t="s">
-        <v>117</v>
+        <v>172</v>
       </c>
       <c r="G86" s="14" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="H86" s="7"/>
+    </row>
+    <row r="87" spans="1:8" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
         <v>86</v>
       </c>
@@ -3552,7 +3558,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="88" spans="1:8" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
         <v>164</v>
       </c>
@@ -3576,8 +3582,42 @@
         <v>138</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C89" s="7"/>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E89" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F89" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G89" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="H89" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="C90" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="E90" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="F90" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="G90" s="14" t="s">
+        <v>89</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3587,18 +3627,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3779,18 +3819,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC4DE233-B05C-40D4-9E0D-B697BD35B3E3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B8261F5-E2C2-49F8-99F3-13EB69507EB7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B8261F5-E2C2-49F8-99F3-13EB69507EB7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC4DE233-B05C-40D4-9E0D-B697BD35B3E3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Added RL and Estimated flags across all water chem studies
</commit_message>
<xml_diff>
--- a/Meta/flagsMap_withDecisions.xlsx
+++ b/Meta/flagsMap_withDecisions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/vitense_kelsey_epa_gov/Documents/GL_Data/Meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="461" documentId="13_ncr:4000b_{6437034B-B068-4CF2-9A04-9208A97A6BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12D9D468-7F45-425A-9914-E4483D48E857}"/>
+  <xr:revisionPtr revIDLastSave="502" documentId="13_ncr:4000b_{6437034B-B068-4CF2-9A04-9208A97A6BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{24206FD2-CA27-4C65-851A-9C8B396803E8}"/>
   <bookViews>
-    <workbookView xWindow="-61548" yWindow="-1872" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25710" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="flagsMap_withDecisions" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
     Note: Did not include 3 extra flags in current flagsMap.csv here with repeat QAcomment in QAcode</t>
       </text>
     </comment>
-    <comment ref="A11" authorId="4" shapeId="0" xr:uid="{A8BE5C20-40BD-42DF-838C-01B7D5AFF883}">
+    <comment ref="A20" authorId="4" shapeId="0" xr:uid="{A8BE5C20-40BD-42DF-838C-01B7D5AFF883}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -81,7 +81,7 @@
     In current flagsMap.csv, did not include R-no reported units because should go with U (row 47). Did not include Q10,R-recorded mean secchi depth is greater than station depth because it's for NC, not GL.</t>
       </text>
     </comment>
-    <comment ref="A34" authorId="5" shapeId="0" xr:uid="{6A749074-B681-48EE-9D60-AAD094A450F9}">
+    <comment ref="A43" authorId="5" shapeId="0" xr:uid="{6A749074-B681-48EE-9D60-AAD094A450F9}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="181">
   <si>
     <t>Study</t>
   </si>
@@ -588,9 +588,6 @@
     <t>MDL imputed</t>
   </si>
   <si>
-    <t>CSMI_2021</t>
-  </si>
-  <si>
     <t>F</t>
   </si>
   <si>
@@ -625,6 +622,21 @@
   </si>
   <si>
     <t>time imputed as noon</t>
+  </si>
+  <si>
+    <t>CSMI_2021_WQ</t>
+  </si>
+  <si>
+    <t>RL</t>
+  </si>
+  <si>
+    <t>below RL</t>
+  </si>
+  <si>
+    <t>Set value to NA; report RL in separate column</t>
+  </si>
+  <si>
+    <t>between MDL and RL</t>
   </si>
 </sst>
 </file>
@@ -1573,10 +1585,10 @@
   <threadedComment ref="A6" dT="2024-08-14T17:05:26.53" personId="{661D028C-1F83-4763-B7EC-DB616DE23CF1}" id="{907734F2-7127-48D9-8E0B-8B1C2E203CA7}">
     <text>Note: Did not include 3 extra flags in current flagsMap.csv here with repeat QAcomment in QAcode</text>
   </threadedComment>
-  <threadedComment ref="A11" dT="2024-08-14T17:33:35.12" personId="{661D028C-1F83-4763-B7EC-DB616DE23CF1}" id="{A8BE5C20-40BD-42DF-838C-01B7D5AFF883}">
+  <threadedComment ref="A20" dT="2024-08-14T17:33:35.12" personId="{661D028C-1F83-4763-B7EC-DB616DE23CF1}" id="{A8BE5C20-40BD-42DF-838C-01B7D5AFF883}">
     <text>In current flagsMap.csv, did not include R-no reported units because should go with U (row 47). Did not include Q10,R-recorded mean secchi depth is greater than station depth because it's for NC, not GL.</text>
   </threadedComment>
-  <threadedComment ref="A34" dT="2024-08-14T17:05:26.53" personId="{661D028C-1F83-4763-B7EC-DB616DE23CF1}" id="{6A749074-B681-48EE-9D60-AAD094A450F9}">
+  <threadedComment ref="A43" dT="2024-08-14T17:05:26.53" personId="{661D028C-1F83-4763-B7EC-DB616DE23CF1}" id="{6A749074-B681-48EE-9D60-AAD094A450F9}">
     <text>Note: Did not include 3 extra flags in current flagsMap.csv here with repeat QAcomment in QAcode</text>
   </threadedComment>
 </ThreadedComments>
@@ -1584,26 +1596,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T90"/>
+  <dimension ref="A1:T99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="44.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="38.5703125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="44.33203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="38.5546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="15" style="6" customWidth="1"/>
     <col min="6" max="6" width="26" style="6" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="35.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="6"/>
+    <col min="7" max="7" width="10.5546875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="35.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1629,24 +1641,24 @@
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>30</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G2" s="13" t="s">
         <v>132</v>
@@ -1655,24 +1667,24 @@
         <v>138</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>86</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>30</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G3" s="13" t="s">
         <v>132</v>
@@ -1681,24 +1693,24 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>52</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>30</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G4" s="13" t="s">
         <v>132</v>
@@ -1707,24 +1719,24 @@
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+    <row r="5" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
         <v>50</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>30</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G5" s="13" t="s">
         <v>132</v>
@@ -1733,24 +1745,24 @@
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>30</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G6" s="13" t="s">
         <v>132</v>
@@ -1759,24 +1771,24 @@
         <v>138</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>27</v>
+        <v>174</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>168</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>30</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G7" s="13" t="s">
         <v>132</v>
@@ -1785,267 +1797,301 @@
         <v>138</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>23</v>
+    <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>176</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>166</v>
+        <v>129</v>
       </c>
       <c r="G8" s="13" t="s">
         <v>132</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>4</v>
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>86</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>166</v>
+        <v>129</v>
       </c>
       <c r="G9" s="13" t="s">
         <v>132</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>166</v>
+        <v>129</v>
       </c>
       <c r="G10" s="13" t="s">
         <v>132</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="B12" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F12" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>4</v>
+        <v>174</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>5</v>
+        <v>177</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>177</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>6</v>
+        <v>178</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>6</v>
+        <v>15</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>129</v>
       </c>
       <c r="G13" s="13" t="s">
         <v>132</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>4</v>
+        <v>179</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>176</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>8</v>
+        <v>128</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>180</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>4</v>
+        <v>94</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>86</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>9</v>
+        <v>128</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>10</v>
+        <v>128</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>11</v>
+        <v>180</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>128</v>
       </c>
       <c r="G15" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="H15" s="7" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>9</v>
+        <v>128</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>12</v>
+        <v>128</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>11</v>
+        <v>180</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>128</v>
       </c>
       <c r="G16" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="H16" s="7" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>4</v>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>50</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>21</v>
+        <v>128</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="H17" s="7"/>
-    </row>
-    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>9</v>
+        <v>128</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>13</v>
+        <v>128</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="H18" s="7"/>
-    </row>
-    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>4</v>
+        <v>174</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>9</v>
+        <v>128</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>14</v>
+        <v>128</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G19" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="H19" s="7"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>4</v>
       </c>
@@ -2053,858 +2099,807 @@
         <v>18</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>149</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="7"/>
       <c r="G20" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="H20" s="11"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>149</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="7"/>
       <c r="G21" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="H21" s="11"/>
-    </row>
-    <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="H21" s="7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G24" s="12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B25" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G25" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B25" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B26" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="H26" s="7"/>
+    </row>
+    <row r="27" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C27" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="H27" s="7"/>
+    </row>
+    <row r="28" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="H28" s="7"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="H29" s="11"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="H30" s="11"/>
+    </row>
+    <row r="31" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A33" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G33" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G34" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G26" s="15" t="s">
+      <c r="G35" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="H26" s="11" t="s">
+      <c r="H35" s="11" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B36" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C36" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D36" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="E36" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="F36" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="G27" s="16" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
+      <c r="G36" s="16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B37" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C37" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D37" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="E37" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="F28" s="6" t="s">
+      <c r="F37" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="G28" s="16" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+      <c r="G37" s="16" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C38" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G29" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="H29" s="6" t="s">
+      <c r="G38" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A39" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G39" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="H39" s="6" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+    <row r="40" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C30" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G30" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="H30" s="6" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B31" s="6" t="s">
+      <c r="B40" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C40" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D40" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E31" s="6" t="s">
+      <c r="E40" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F31" s="6" t="s">
+      <c r="F40" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="G31" s="13" t="s">
+      <c r="G40" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="H31" s="6" t="s">
+      <c r="H40" s="6" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="6" t="s">
+    <row r="41" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A41" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B41" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C41" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D41" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E32" s="6" t="s">
+      <c r="E41" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F32" s="6" t="s">
+      <c r="F41" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="G32" s="13" t="s">
+      <c r="G41" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="H32" s="6" t="s">
+      <c r="H41" s="6" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B42" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C42" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E33" s="6" t="s">
+      <c r="E42" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F33" s="6" t="s">
+      <c r="F42" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G33" s="13" t="s">
+      <c r="G42" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="H33" s="6" t="s">
+      <c r="H42" s="6" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
+    <row r="43" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A43" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B43" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C43" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="D43" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E34" s="7" t="s">
+      <c r="E43" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F34" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="G34" s="13" t="s">
+      <c r="F43" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="G43" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="H34" s="6" t="s">
+      <c r="H43" s="6" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
+    <row r="44" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B44" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C44" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="D44" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E35" s="6" t="s">
+      <c r="E44" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="F35" s="6" t="s">
+      <c r="F44" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="G35" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="H35" s="7"/>
-    </row>
-    <row r="36" spans="1:20" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
+      <c r="G44" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="H44" s="7"/>
+    </row>
+    <row r="45" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A45" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B45" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C45" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="D45" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E36" s="7" t="s">
+      <c r="E45" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F36" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="G36" s="13" t="s">
+      <c r="F45" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="G45" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="H36" s="6" t="s">
+      <c r="H45" s="6" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="6" t="s">
+    <row r="46" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B46" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C46" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="D46" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E37" s="7" t="s">
+      <c r="E46" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="F37" s="7" t="s">
+      <c r="F46" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="G37" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
+      <c r="G46" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B47" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C47" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E38" s="6" t="s">
+      <c r="E47" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="F38" s="6" t="s">
+      <c r="F47" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="G38" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="6" t="s">
+      <c r="G47" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B48" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C48" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="D48" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E39" s="6" t="s">
+      <c r="E48" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="F39" s="1" t="s">
+      <c r="F48" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G39" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="6" t="s">
+      <c r="G48" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A49" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B49" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C49" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="G40" s="15" t="s">
+      <c r="G49" s="15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="6" t="s">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A50" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B41" s="6" t="s">
+      <c r="B50" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C41" s="6" t="s">
+      <c r="C50" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="D50" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G41" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="H41" s="7" t="s">
+      <c r="G50" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="H50" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
+    <row r="51" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A51" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B51" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C51" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E42" s="6" t="s">
+      <c r="E51" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="F42" s="6" t="s">
+      <c r="F51" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="G42" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20" s="7" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A43" s="10" t="s">
+      <c r="G51" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" s="7" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A52" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="B52" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C43" s="8" t="s">
+      <c r="C52" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="D43" s="9"/>
-      <c r="E43" s="10" t="s">
+      <c r="D52" s="9"/>
+      <c r="E52" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="F52" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="G52" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="H52" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" s="10" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A53" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="D53" s="5"/>
+      <c r="E53" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F53" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="F43" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="G43" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="H43" s="7" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="44" spans="1:20" s="10" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A44" s="7" t="s">
+      <c r="G53" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="H53" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="I53" s="7"/>
+      <c r="J53" s="7"/>
+      <c r="K53" s="7"/>
+      <c r="L53" s="7"/>
+      <c r="M53" s="7"/>
+      <c r="N53" s="7"/>
+      <c r="O53" s="7"/>
+      <c r="P53" s="7"/>
+      <c r="Q53" s="7"/>
+      <c r="R53" s="7"/>
+      <c r="S53" s="7"/>
+      <c r="T53" s="7"/>
+    </row>
+    <row r="54" spans="1:20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>50</v>
       </c>
-      <c r="B44" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="D44" s="5"/>
-      <c r="E44" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="G44" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="H44" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="I44" s="7"/>
-      <c r="J44" s="7"/>
-      <c r="K44" s="7"/>
-      <c r="L44" s="7"/>
-      <c r="M44" s="7"/>
-      <c r="N44" s="7"/>
-      <c r="O44" s="7"/>
-      <c r="P44" s="7"/>
-      <c r="Q44" s="7"/>
-      <c r="R44" s="7"/>
-      <c r="S44" s="7"/>
-      <c r="T44" s="7"/>
-    </row>
-    <row r="45" spans="1:20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="B54" t="s">
+        <v>93</v>
+      </c>
+      <c r="C54" t="s">
+        <v>155</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="G54" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>50</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B55" t="s">
         <v>93</v>
       </c>
-      <c r="C45" t="s">
-        <v>155</v>
-      </c>
-      <c r="D45" s="7" t="s">
+      <c r="C55" t="s">
+        <v>156</v>
+      </c>
+      <c r="D55" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="E45" s="7" t="s">
+      <c r="E55" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="F45" s="7" t="s">
+      <c r="F55" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="G45" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="46" spans="1:20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="G55" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>50</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B56" t="s">
         <v>93</v>
       </c>
-      <c r="C46" t="s">
-        <v>156</v>
-      </c>
-      <c r="D46" s="7" t="s">
+      <c r="C56" t="s">
+        <v>157</v>
+      </c>
+      <c r="D56" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="E46" s="7" t="s">
+      <c r="E56" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="F46" s="7" t="s">
+      <c r="F56" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="G46" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="47" spans="1:20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="G56" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
         <v>50</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B57" t="s">
         <v>93</v>
       </c>
-      <c r="C47" t="s">
-        <v>157</v>
-      </c>
-      <c r="D47" s="7" t="s">
+      <c r="C57" t="s">
+        <v>158</v>
+      </c>
+      <c r="D57" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="E47" s="7" t="s">
+      <c r="E57" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="F47" s="7" t="s">
+      <c r="F57" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="G47" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="48" spans="1:20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="G57" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
         <v>50</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B58" t="s">
         <v>93</v>
       </c>
-      <c r="C48" t="s">
-        <v>158</v>
-      </c>
-      <c r="D48" s="7" t="s">
+      <c r="C58" t="s">
+        <v>159</v>
+      </c>
+      <c r="D58" s="7" t="s">
         <v>134</v>
-      </c>
-      <c r="E48" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="F48" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="G48" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="49" spans="1:20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>50</v>
-      </c>
-      <c r="B49" t="s">
-        <v>93</v>
-      </c>
-      <c r="C49" t="s">
-        <v>159</v>
-      </c>
-      <c r="D49" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="G49" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="50" spans="1:20" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="G50" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="H50" s="7"/>
-      <c r="I50" s="7"/>
-      <c r="J50" s="7"/>
-      <c r="K50" s="7"/>
-      <c r="L50" s="7"/>
-      <c r="M50" s="7"/>
-      <c r="N50" s="7"/>
-      <c r="O50" s="7"/>
-      <c r="P50" s="7"/>
-      <c r="Q50" s="7"/>
-      <c r="R50" s="7"/>
-      <c r="S50" s="7"/>
-      <c r="T50" s="7"/>
-    </row>
-    <row r="51" spans="1:20" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C51" s="7"/>
-      <c r="D51" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="E51" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="F51" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G51" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="H51" s="7"/>
-      <c r="I51" s="7"/>
-      <c r="J51" s="7"/>
-      <c r="K51" s="7"/>
-      <c r="L51" s="7"/>
-      <c r="M51" s="7"/>
-      <c r="N51" s="7"/>
-      <c r="O51" s="7"/>
-      <c r="P51" s="7"/>
-      <c r="Q51" s="7"/>
-      <c r="R51" s="7"/>
-      <c r="S51" s="7"/>
-      <c r="T51" s="7"/>
-    </row>
-    <row r="52" spans="1:20" ht="45.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B52" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C52" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E52" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F52" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="G52" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="H52" s="7"/>
-    </row>
-    <row r="53" spans="1:20" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C53" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E53" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F53" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="G53" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="54" spans="1:20" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A54" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C54" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E54" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G54" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="55" spans="1:20" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A55" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C55" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E55" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F55" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="G55" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="56" spans="1:20" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A56" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C56" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="E56" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F56" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="G56" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="57" spans="1:20" ht="165" x14ac:dyDescent="0.25">
-      <c r="A57" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C57" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E57" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F57" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="G57" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="H57" s="7" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="58" spans="1:20" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A58" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C58" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="E58" s="7" t="s">
         <v>93</v>
@@ -2916,53 +2911,75 @@
         <v>89</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="A59" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C59" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>105</v>
-      </c>
+    <row r="59" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D59" s="7"/>
       <c r="E59" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="G59" s="14" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="60" spans="1:20" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A60" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C60" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>95</v>
+      <c r="H59" s="7"/>
+      <c r="I59" s="7"/>
+      <c r="J59" s="7"/>
+      <c r="K59" s="7"/>
+      <c r="L59" s="7"/>
+      <c r="M59" s="7"/>
+      <c r="N59" s="7"/>
+      <c r="O59" s="7"/>
+      <c r="P59" s="7"/>
+      <c r="Q59" s="7"/>
+      <c r="R59" s="7"/>
+      <c r="S59" s="7"/>
+      <c r="T59" s="7"/>
+    </row>
+    <row r="60" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C60" s="7"/>
+      <c r="D60" s="7" t="s">
+        <v>133</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>128</v>
+        <v>41</v>
       </c>
       <c r="G60" s="14" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="61" spans="1:20" ht="60" x14ac:dyDescent="0.25">
+      <c r="H60" s="7"/>
+      <c r="I60" s="7"/>
+      <c r="J60" s="7"/>
+      <c r="K60" s="7"/>
+      <c r="L60" s="7"/>
+      <c r="M60" s="7"/>
+      <c r="N60" s="7"/>
+      <c r="O60" s="7"/>
+      <c r="P60" s="7"/>
+      <c r="Q60" s="7"/>
+      <c r="R60" s="7"/>
+      <c r="S60" s="7"/>
+      <c r="T60" s="7"/>
+    </row>
+    <row r="61" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A61" s="6" t="s">
         <v>52</v>
       </c>
@@ -2970,25 +2987,23 @@
         <v>53</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="E61" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F61" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="G61" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="H61" s="7" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="62" spans="1:20" ht="34.5" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F61" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G61" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="H61" s="7"/>
+    </row>
+    <row r="62" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A62" s="6" t="s">
         <v>52</v>
       </c>
@@ -2996,10 +3011,10 @@
         <v>53</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="E62" s="6" t="s">
         <v>93</v>
@@ -3011,7 +3026,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="63" spans="1:20" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A63" s="6" t="s">
         <v>52</v>
       </c>
@@ -3019,22 +3034,22 @@
         <v>53</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F63" s="6" t="s">
-        <v>117</v>
+        <v>92</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="G63" s="14" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="64" spans="1:20" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A64" s="6" t="s">
         <v>52</v>
       </c>
@@ -3042,22 +3057,22 @@
         <v>53</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>144</v>
+        <v>93</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="G64" s="14" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A65" s="6" t="s">
         <v>52</v>
       </c>
@@ -3065,10 +3080,10 @@
         <v>53</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="E65" s="6" t="s">
         <v>93</v>
@@ -3080,7 +3095,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A66" s="6" t="s">
         <v>52</v>
       </c>
@@ -3088,22 +3103,25 @@
         <v>53</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="E66" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F66" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="G66" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="E66" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F66" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="G66" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="H66" s="7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A67" s="6" t="s">
         <v>52</v>
       </c>
@@ -3111,16 +3129,22 @@
         <v>53</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G67" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="E67" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F67" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="G67" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A68" s="6" t="s">
         <v>52</v>
       </c>
@@ -3128,22 +3152,22 @@
         <v>53</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E68" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E68" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="F68" s="6" t="s">
+      <c r="F68" s="7" t="s">
         <v>117</v>
       </c>
       <c r="G68" s="14" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="45.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A69" s="6" t="s">
         <v>52</v>
       </c>
@@ -3151,25 +3175,22 @@
         <v>53</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>15</v>
+        <v>94</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="G69" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="H69" s="7" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+      <c r="G69" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A70" s="6" t="s">
         <v>52</v>
       </c>
@@ -3177,22 +3198,25 @@
         <v>53</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E70" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F70" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="G70" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="E70" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="F70" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="G70" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="H70" s="7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A71" s="6" t="s">
         <v>52</v>
       </c>
@@ -3200,10 +3224,10 @@
         <v>53</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>115</v>
+        <v>64</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>107</v>
       </c>
       <c r="E71" s="6" t="s">
         <v>93</v>
@@ -3215,7 +3239,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A72" s="6" t="s">
         <v>52</v>
       </c>
@@ -3223,16 +3247,22 @@
         <v>53</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="G72" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" ht="57" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E72" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F72" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G72" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A73" s="6" t="s">
         <v>52</v>
       </c>
@@ -3240,22 +3270,22 @@
         <v>53</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>118</v>
+        <v>66</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>93</v>
+        <v>144</v>
       </c>
       <c r="F73" s="6" t="s">
-        <v>117</v>
+        <v>145</v>
       </c>
       <c r="G73" s="14" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A74" s="6" t="s">
         <v>52</v>
       </c>
@@ -3263,10 +3293,10 @@
         <v>53</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="D74" s="3" t="s">
-        <v>119</v>
+        <v>67</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>110</v>
       </c>
       <c r="E74" s="6" t="s">
         <v>93</v>
@@ -3278,7 +3308,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A75" s="6" t="s">
         <v>52</v>
       </c>
@@ -3286,25 +3316,22 @@
         <v>53</v>
       </c>
       <c r="C75" s="6" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="E75" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F75" s="7" t="s">
-        <v>128</v>
+        <v>111</v>
+      </c>
+      <c r="E75" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F75" s="6" t="s">
+        <v>117</v>
       </c>
       <c r="G75" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="H75" s="7" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:8" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A76" s="6" t="s">
         <v>52</v>
       </c>
@@ -3312,22 +3339,16 @@
         <v>53</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="E76" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="F76" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="G76" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="G76" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="21.6" x14ac:dyDescent="0.3">
       <c r="A77" s="6" t="s">
         <v>52</v>
       </c>
@@ -3335,10 +3356,10 @@
         <v>53</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D77" s="3" t="s">
-        <v>121</v>
+        <v>70</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>113</v>
       </c>
       <c r="E77" s="6" t="s">
         <v>93</v>
@@ -3350,7 +3371,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A78" s="6" t="s">
         <v>52</v>
       </c>
@@ -3358,22 +3379,25 @@
         <v>53</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>122</v>
+        <v>71</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>98</v>
       </c>
       <c r="E78" s="7" t="s">
-        <v>94</v>
+        <v>15</v>
       </c>
       <c r="F78" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="G78" s="14" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="G78" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="H78" s="7" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="52.2" x14ac:dyDescent="0.3">
       <c r="A79" s="6" t="s">
         <v>52</v>
       </c>
@@ -3381,18 +3405,22 @@
         <v>53</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="E79" s="7"/>
-      <c r="F79" s="7"/>
-      <c r="G79" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E79" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F79" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G79" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A80" s="6" t="s">
         <v>52</v>
       </c>
@@ -3400,22 +3428,22 @@
         <v>53</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="E80" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F80" s="7" t="s">
-        <v>128</v>
+        <v>115</v>
+      </c>
+      <c r="E80" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F80" s="6" t="s">
+        <v>117</v>
       </c>
       <c r="G80" s="14" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A81" s="6" t="s">
         <v>52</v>
       </c>
@@ -3423,16 +3451,16 @@
         <v>53</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="G81" s="15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="45.75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" ht="42" x14ac:dyDescent="0.3">
       <c r="A82" s="6" t="s">
         <v>52</v>
       </c>
@@ -3440,10 +3468,10 @@
         <v>53</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="E82" s="6" t="s">
         <v>93</v>
@@ -3455,7 +3483,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A83" s="6" t="s">
         <v>52</v>
       </c>
@@ -3463,16 +3491,22 @@
         <v>53</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>146</v>
+        <v>76</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="G83" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="E83" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F83" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G83" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A84" s="6" t="s">
         <v>52</v>
       </c>
@@ -3480,14 +3514,25 @@
         <v>53</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="D84" s="3"/>
-      <c r="G84" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" ht="34.5" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E84" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F84" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G84" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="H84" s="7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A85" s="6" t="s">
         <v>52</v>
       </c>
@@ -3495,10 +3540,10 @@
         <v>53</v>
       </c>
       <c r="C85" s="6" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="E85" s="6" t="s">
         <v>93</v>
@@ -3510,7 +3555,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
       <c r="A86" s="6" t="s">
         <v>52</v>
       </c>
@@ -3518,104 +3563,287 @@
         <v>53</v>
       </c>
       <c r="C86" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E86" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F86" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G86" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
+      <c r="A87" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E87" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F87" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G87" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
+      <c r="A88" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B88" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E88" s="7"/>
+      <c r="F88" s="7"/>
+      <c r="G88" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" ht="21.6" x14ac:dyDescent="0.3">
+      <c r="A89" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C89" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E89" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F89" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="G89" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
+      <c r="A90" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C90" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G90" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" ht="42" x14ac:dyDescent="0.3">
+      <c r="A91" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B91" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C91" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E91" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F91" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G91" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A92" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B92" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C92" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="G92" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A93" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B93" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C93" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="D93" s="3"/>
+      <c r="G93" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="31.8" x14ac:dyDescent="0.3">
+      <c r="A94" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B94" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C94" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E94" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F94" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G94" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="21.6" x14ac:dyDescent="0.3">
+      <c r="A95" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B95" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C95" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="D95" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="D86" s="2" t="s">
+      <c r="E95" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="E86" s="6" t="s">
+      <c r="F95" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="F86" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="G86" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="H86" s="7"/>
-    </row>
-    <row r="87" spans="1:8" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A87" s="7" t="s">
+      <c r="G95" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="H95" s="7"/>
+    </row>
+    <row r="96" spans="1:8" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A96" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="B87" s="7" t="s">
+      <c r="B96" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C87" s="7" t="s">
+      <c r="C96" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D87" s="5"/>
-      <c r="E87" s="7" t="s">
+      <c r="D96" s="5"/>
+      <c r="E96" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F87" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="G87" s="13" t="s">
+      <c r="F96" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="G96" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="H87" s="7" t="s">
+      <c r="H96" s="7" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="88" spans="1:8" s="7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A88" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="B88" s="7" t="s">
+    <row r="97" spans="1:8" s="7" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A97" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="B97" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C88" s="7" t="s">
+      <c r="C97" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D88" s="5"/>
-      <c r="E88" s="7" t="s">
+      <c r="D97" s="5"/>
+      <c r="E97" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F88" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="G88" s="13" t="s">
+      <c r="F97" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="G97" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="H88" s="7" t="s">
+      <c r="H97" s="7" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" s="6" t="s">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A98" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="B98" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E98" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F98" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G98" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="H98" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A99" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C99" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="B89" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E89" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F89" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G89" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="H89" s="6" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="C90" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="E90" s="6" t="s">
+      <c r="E99" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="F99" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="F90" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="G90" s="14" t="s">
+      <c r="G99" s="14" t="s">
         <v>89</v>
       </c>
     </row>
@@ -3627,18 +3855,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3819,18 +4047,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B8261F5-E2C2-49F8-99F3-13EB69507EB7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC4DE233-B05C-40D4-9E0D-B697BD35B3E3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC4DE233-B05C-40D4-9E0D-B697BD35B3E3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B8261F5-E2C2-49F8-99F3-13EB69507EB7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Added D flag for imputing depth for CSMI 2021 CTD
</commit_message>
<xml_diff>
--- a/Meta/flagsMap_withDecisions.xlsx
+++ b/Meta/flagsMap_withDecisions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/coffman_christian_epa_gov/Documents/Profile/Documents/Projects/GL_Data/Meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="637" documentId="13_ncr:4000b_{6437034B-B068-4CF2-9A04-9208A97A6BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC139834-6264-4F35-B141-952FCF741899}"/>
+  <xr:revisionPtr revIDLastSave="639" documentId="13_ncr:4000b_{6437034B-B068-4CF2-9A04-9208A97A6BAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16CC6726-41C7-4606-97FD-2D7CCD12AF1A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">flagsMap_withDecisions!$A$1:$A$112</definedName>
   </definedNames>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -97,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17107" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17108" uniqueCount="193">
   <si>
     <t>Study</t>
   </si>
@@ -666,9 +666,6 @@
     <t>NRR</t>
   </si>
   <si>
-    <t>No result reported</t>
-  </si>
-  <si>
     <t>W</t>
   </si>
   <si>
@@ -676,6 +673,9 @@
   </si>
   <si>
     <t>station Depth estimated as the maximum sample Depth</t>
+  </si>
+  <si>
+    <t>no result reported</t>
   </si>
 </sst>
 </file>
@@ -1653,7 +1653,7 @@
   <dimension ref="A1:XFD115"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A102" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D115" sqref="D115"/>
+      <selection activeCell="E114" sqref="E114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3791,7 +3791,7 @@
         <v>53</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="D94" s="3"/>
       <c r="E94" s="7"/>
@@ -53282,7 +53282,7 @@
         <v>52</v>
       </c>
       <c r="C112" s="6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D112" s="2"/>
       <c r="G112" s="14" t="s">
@@ -53292,15 +53292,18 @@
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A113" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B113" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C113" s="18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D113" s="2"/>
+      <c r="E113" s="6" t="s">
+        <v>180</v>
+      </c>
       <c r="G113" s="13" t="s">
         <v>132</v>
       </c>
@@ -53317,7 +53320,7 @@
       <c r="A115" s="7"/>
       <c r="B115"/>
       <c r="C115" s="17" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D115"/>
       <c r="G115" s="19"/>
@@ -53331,18 +53334,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -53523,18 +53526,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B8261F5-E2C2-49F8-99F3-13EB69507EB7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC4DE233-B05C-40D4-9E0D-B697BD35B3E3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AC4DE233-B05C-40D4-9E0D-B697BD35B3E3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B8261F5-E2C2-49F8-99F3-13EB69507EB7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>